<commit_message>
* Added more data processing * Added Lightgbm model * Added more training result
</commit_message>
<xml_diff>
--- a/training_result.xlsx
+++ b/training_result.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="31095" yWindow="0" windowWidth="19305" windowHeight="8340"/>
+    <workbookView xWindow="2895" yWindow="0" windowWidth="18690" windowHeight="11685"/>
   </bookViews>
   <sheets>
     <sheet name="kernel_private" sheetId="6" r:id="rId1"/>
     <sheet name="kernel1_public" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr autoRecover="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="49">
   <si>
     <t>Model</t>
   </si>
@@ -125,10 +126,6 @@
   </si>
   <si>
     <t>fill NA, LabelEncoder, add features, remove features,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">kernel name: TBD
-</t>
   </si>
   <si>
     <t>2985217,56</t>
@@ -153,12 +150,72 @@
     <t>+ above
 + remove outliers: finishedsquarefeet15(&gt;20000), garagecarcnt(&gt;20), garagetotalsqft(&gt;6000), lotsizesquarefeet(&gt;6000000), poolsizesum(&gt;1500), unitcnt(&gt;60), taxdelinquencyyear(&gt;80)</t>
   </si>
+  <si>
+    <t>80133,56</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8382,56</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>+ eta: 0.007
++ max_depth: 7
++ subsample: 0.6
++ lambda: 5.0
++ alpha: 0.65
++ bytree: 0.5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>+ above
++ train: [-0.4, 0.419]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>+ above
++ remove outliers based on correlation: 'poolsizesum', 'storytypeid', 'typeconstructiontypeid', 'decktypeid', 'pooltypeid10',</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>+ above
++ add fts: add_features()
++ remove fts: select_features()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>too many features ==&gt; overfitting</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>+ above
++ add fts: just added high-correlation features
++ remove fts: poolsizesum, pooltypeid10, decktypeid, pooltypeid2, architecturalstyletypeid, storytypeid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>inherited from r8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>+ as (4)
++ add fts: N-zip_count, N-city_count, N-GarPoolAC, mean_area, med_year, med_lat, med_long
++ remove fts: regionidcounty, poolsizesum, yardbuildingsqft26, decktypeid, storytypeid, pooltypeid2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kernel name: xgboost version 2</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -217,6 +274,32 @@
       <color rgb="FF3333CC"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3333CC"/>
+      <name val="Calibri"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="3"/>
+      <charset val="129"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -280,7 +363,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -351,23 +434,32 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -661,19 +753,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D4" sqref="D4"/>
+      <selection pane="topRight" activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="6" style="17" customWidth="1"/>
-    <col min="2" max="2" width="62.5703125" style="17" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" style="17" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" style="17" customWidth="1"/>
+    <col min="2" max="2" width="70.85546875" style="17" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" style="17" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" style="17" customWidth="1"/>
     <col min="5" max="5" width="10.85546875" style="17" customWidth="1"/>
     <col min="6" max="6" width="8.42578125" style="17" customWidth="1"/>
     <col min="7" max="7" width="12" style="17" customWidth="1"/>
@@ -683,10 +775,10 @@
     <col min="11" max="16384" width="9.140625" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="25" customFormat="1" ht="25.5" customHeight="1">
+    <row r="1" spans="1:11" s="24" customFormat="1" ht="25.5" customHeight="1">
       <c r="A1" s="23"/>
-      <c r="B1" s="24" t="s">
-        <v>33</v>
+      <c r="B1" s="32" t="s">
+        <v>48</v>
       </c>
       <c r="C1" s="23"/>
       <c r="D1" s="23"/>
@@ -697,7 +789,7 @@
       <c r="I1" s="23"/>
       <c r="J1" s="23"/>
     </row>
-    <row r="2" spans="1:10" ht="5.25" customHeight="1">
+    <row r="2" spans="1:11" ht="5.25" customHeight="1">
       <c r="A2" s="19"/>
       <c r="B2" s="16"/>
       <c r="C2" s="19"/>
@@ -709,7 +801,7 @@
       <c r="I2" s="19"/>
       <c r="J2" s="19"/>
     </row>
-    <row r="3" spans="1:10" ht="30" customHeight="1">
+    <row r="3" spans="1:11" ht="30" customHeight="1">
       <c r="A3" s="4" t="s">
         <v>17</v>
       </c>
@@ -741,18 +833,18 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="19" customFormat="1" ht="89.25">
+    <row r="4" spans="1:11" s="19" customFormat="1" ht="78.75">
       <c r="A4" s="11">
         <v>1</v>
       </c>
-      <c r="B4" s="26" t="s">
-        <v>35</v>
+      <c r="B4" s="25" t="s">
+        <v>34</v>
       </c>
       <c r="C4" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="27" t="s">
-        <v>36</v>
+      <c r="D4" s="25" t="s">
+        <v>35</v>
       </c>
       <c r="E4" s="13" t="s">
         <v>30</v>
@@ -761,24 +853,24 @@
         <v>31</v>
       </c>
       <c r="G4" s="19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H4" s="19">
         <v>5.1650000000000001E-2</v>
       </c>
-      <c r="I4" s="29">
+      <c r="I4" s="26">
         <v>6.4611000000000002E-2</v>
       </c>
       <c r="J4" s="19">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="19" customFormat="1" ht="51">
+    <row r="5" spans="1:11" s="19" customFormat="1" ht="33.75">
       <c r="A5" s="19">
         <v>2</v>
       </c>
-      <c r="B5" s="28" t="s">
-        <v>37</v>
+      <c r="B5" s="27" t="s">
+        <v>36</v>
       </c>
       <c r="C5" s="18" t="s">
         <v>23</v>
@@ -798,32 +890,184 @@
       <c r="H5" s="18">
         <v>5.1652999999999998E-2</v>
       </c>
-      <c r="I5" s="29">
+      <c r="I5" s="26">
         <v>6.4565600000000001E-2</v>
       </c>
       <c r="J5" s="19">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
-      <c r="B6" s="22"/>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="B7" s="22"/>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="B8" s="22"/>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="B9" s="22"/>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="B10" s="22"/>
-    </row>
-    <row r="11" spans="1:10">
+    <row r="6" spans="1:11" ht="67.5">
+      <c r="A6" s="19">
+        <v>3</v>
+      </c>
+      <c r="B6" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6" s="18">
+        <v>5.1644000000000002E-2</v>
+      </c>
+      <c r="I6" s="26">
+        <v>6.4564800000000006E-2</v>
+      </c>
+      <c r="J6" s="19">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="33.75">
+      <c r="A7" s="19">
+        <v>4</v>
+      </c>
+      <c r="B7" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="G7" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7" s="18">
+        <v>5.1604999999999998E-2</v>
+      </c>
+      <c r="I7" s="26">
+        <v>6.4559000000000005E-2</v>
+      </c>
+      <c r="J7" s="19">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="33.75">
+      <c r="A8" s="19">
+        <v>5</v>
+      </c>
+      <c r="B8" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="G8" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="H8" s="17">
+        <v>5.1681999999999999E-2</v>
+      </c>
+      <c r="I8" s="28">
+        <v>6.4625600000000005E-2</v>
+      </c>
+      <c r="J8" s="17">
+        <v>9</v>
+      </c>
+      <c r="K8" s="29" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="45">
+      <c r="A9" s="19">
+        <v>6</v>
+      </c>
+      <c r="B9" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="G9" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="H9" s="21">
+        <v>5.1711E-2</v>
+      </c>
+      <c r="I9" s="28">
+        <v>6.4605700000000002E-2</v>
+      </c>
+      <c r="J9" s="21">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="33.75">
+      <c r="A10" s="19">
+        <v>7</v>
+      </c>
+      <c r="B10" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="F10" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="G10" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="H10" s="21">
+        <v>5.1580000000000001E-2</v>
+      </c>
+      <c r="I10" s="30">
+        <v>6.4518699999999998E-2</v>
+      </c>
+      <c r="J10" s="21">
+        <v>12</v>
+      </c>
+      <c r="K10" s="29" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
       <c r="B11" s="22"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -837,7 +1081,7 @@
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="6" style="1" customWidth="1"/>
     <col min="2" max="2" width="28.7109375" style="1" customWidth="1"/>
@@ -1102,10 +1346,10 @@
       <c r="D10" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="21" t="s">
+      <c r="E10" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="F10" s="21"/>
+      <c r="F10" s="31"/>
       <c r="G10" s="14" t="s">
         <v>23</v>
       </c>

</xml_diff>

<commit_message>
* Added full-data train * Added hyperparameter tunning * Updated training result.
</commit_message>
<xml_diff>
--- a/training_result.xlsx
+++ b/training_result.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2895" yWindow="0" windowWidth="18690" windowHeight="11685"/>
+    <workbookView xWindow="5355" yWindow="0" windowWidth="18690" windowHeight="11685"/>
   </bookViews>
   <sheets>
     <sheet name="kernel_private" sheetId="6" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="65">
   <si>
     <t>Model</t>
   </si>
@@ -210,12 +210,71 @@
   <si>
     <t>kernel name: xgboost version 2</t>
   </si>
+  <si>
+    <t>lightgbm</t>
+  </si>
+  <si>
+    <t>+ max_bin: 10
++ learning_rate: 0.0021
++ boosting_type: gbdt
++ metric: mae
++ sub_feature: 0.5
++ fraction: 0.85
++ bagging_freq: 40
++ leaves: 512
++ min_data: 500
++ hessian: 0.05</t>
+  </si>
+  <si>
+    <t>80133,58</t>
+  </si>
+  <si>
+    <t>8382,58</t>
+  </si>
+  <si>
+    <t>2985217,58</t>
+  </si>
+  <si>
+    <t>+ xgboost: 0.6
++ lightgbm: 0.4</t>
+  </si>
+  <si>
+    <t>+ 0.05158
++ 0.0516687</t>
+  </si>
+  <si>
+    <t>xgboost: 0.65</t>
+  </si>
+  <si>
+    <t>+sub_feature(0.2)</t>
+  </si>
+  <si>
+    <t>lightgbm: 0.35</t>
+  </si>
+  <si>
+    <t>xgboost: 0.75</t>
+  </si>
+  <si>
+    <t>lightgbm: 0.25</t>
+  </si>
+  <si>
+    <t>xgboost: 0.85</t>
+  </si>
+  <si>
+    <t>lightgbm: 0.15</t>
+  </si>
+  <si>
+    <t>kernel version</t>
+  </si>
+  <si>
+    <t>github version</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -269,14 +328,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FF3333CC"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="8"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -285,21 +336,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3333CC"/>
+      <sz val="12"/>
       <name val="Calibri"/>
-      <family val="3"/>
-      <charset val="129"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF00B050"/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <family val="3"/>
-      <charset val="129"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -323,7 +369,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -359,11 +405,97 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -425,47 +557,156 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
@@ -753,43 +994,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="6" style="17" customWidth="1"/>
-    <col min="2" max="2" width="70.85546875" style="17" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" style="17" customWidth="1"/>
+    <col min="2" max="2" width="65.28515625" style="17" customWidth="1"/>
+    <col min="3" max="3" width="13" style="17" customWidth="1"/>
     <col min="4" max="4" width="15.42578125" style="17" customWidth="1"/>
     <col min="5" max="5" width="10.85546875" style="17" customWidth="1"/>
     <col min="6" max="6" width="8.42578125" style="17" customWidth="1"/>
     <col min="7" max="7" width="12" style="17" customWidth="1"/>
-    <col min="8" max="8" width="9.85546875" style="17" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" style="17" customWidth="1"/>
     <col min="9" max="9" width="11.28515625" style="17" customWidth="1"/>
-    <col min="10" max="10" width="8.28515625" style="17" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="17"/>
+    <col min="10" max="10" width="7.140625" style="26" customWidth="1"/>
+    <col min="11" max="11" width="8.28515625" style="17" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="24" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A1" s="23"/>
-      <c r="B1" s="32" t="s">
+    <row r="1" spans="1:12" s="22" customFormat="1" ht="27.75" customHeight="1">
+      <c r="A1" s="21"/>
+      <c r="B1" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-    </row>
-    <row r="2" spans="1:11" ht="5.25" customHeight="1">
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+    </row>
+    <row r="2" spans="1:12" ht="2.25" customHeight="1">
       <c r="A2" s="19"/>
       <c r="B2" s="16"/>
       <c r="C2" s="19"/>
@@ -799,9 +1042,10 @@
       <c r="G2" s="19"/>
       <c r="H2" s="19"/>
       <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-    </row>
-    <row r="3" spans="1:11" ht="30" customHeight="1">
+      <c r="J2" s="27"/>
+      <c r="K2" s="19"/>
+    </row>
+    <row r="3" spans="1:12" ht="30" customHeight="1">
       <c r="A3" s="4" t="s">
         <v>17</v>
       </c>
@@ -829,47 +1073,51 @@
       <c r="I3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="J3" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" s="19" customFormat="1" ht="78.75">
-      <c r="A4" s="11">
+      <c r="J3" s="59" t="s">
+        <v>63</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" s="19" customFormat="1" ht="78.75">
+      <c r="A4" s="29">
         <v>1</v>
       </c>
-      <c r="B4" s="25" t="s">
+      <c r="B4" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="25" t="s">
+      <c r="D4" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="F4" s="19" t="s">
+      <c r="F4" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="G4" s="19" t="s">
+      <c r="G4" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="H4" s="19">
+      <c r="H4" s="33">
         <v>5.1650000000000001E-2</v>
       </c>
-      <c r="I4" s="26">
+      <c r="I4" s="34">
         <v>6.4611000000000002E-2</v>
       </c>
-      <c r="J4" s="19">
+      <c r="J4" s="33">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" s="19" customFormat="1" ht="33.75">
+      <c r="K4" s="35"/>
+    </row>
+    <row r="5" spans="1:12" s="19" customFormat="1" ht="33.75">
       <c r="A5" s="19">
         <v>2</v>
       </c>
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="23" t="s">
         <v>36</v>
       </c>
       <c r="C5" s="18" t="s">
@@ -890,184 +1138,438 @@
       <c r="H5" s="18">
         <v>5.1652999999999998E-2</v>
       </c>
-      <c r="I5" s="26">
+      <c r="I5" s="34">
         <v>6.4565600000000001E-2</v>
       </c>
-      <c r="J5" s="19">
+      <c r="J5" s="33">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" ht="67.5">
-      <c r="A6" s="19">
+      <c r="K5" s="35"/>
+    </row>
+    <row r="6" spans="1:12" ht="67.5">
+      <c r="A6" s="36">
         <v>3</v>
       </c>
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="C6" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="25" t="s">
+      <c r="C6" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="E6" s="18" t="s">
+      <c r="E6" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="F6" s="18" t="s">
+      <c r="F6" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="G6" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="H6" s="18">
+      <c r="G6" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6" s="38">
         <v>5.1644000000000002E-2</v>
       </c>
-      <c r="I6" s="26">
+      <c r="I6" s="34">
         <v>6.4564800000000006E-2</v>
       </c>
-      <c r="J6" s="19">
+      <c r="J6" s="33">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" ht="33.75">
-      <c r="A7" s="19">
+      <c r="K6" s="35"/>
+    </row>
+    <row r="7" spans="1:12" ht="33.75">
+      <c r="A7" s="36">
         <v>4</v>
       </c>
-      <c r="B7" s="27" t="s">
+      <c r="B7" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="C7" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="25" t="s">
+      <c r="C7" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="E7" s="18" t="s">
+      <c r="E7" s="38" t="s">
         <v>38</v>
       </c>
-      <c r="F7" s="18" t="s">
+      <c r="F7" s="38" t="s">
         <v>38</v>
       </c>
-      <c r="G7" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="H7" s="18">
+      <c r="G7" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7" s="38">
         <v>5.1604999999999998E-2</v>
       </c>
-      <c r="I7" s="26">
+      <c r="I7" s="34">
         <v>6.4559000000000005E-2</v>
       </c>
-      <c r="J7" s="19">
+      <c r="J7" s="33">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" ht="33.75">
-      <c r="A8" s="19">
+      <c r="K7" s="35"/>
+    </row>
+    <row r="8" spans="1:12" ht="33.75">
+      <c r="A8" s="36">
         <v>5</v>
       </c>
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="25" t="s">
+      <c r="C8" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="E8" s="18" t="s">
+      <c r="E8" s="38" t="s">
         <v>38</v>
       </c>
-      <c r="F8" s="18" t="s">
+      <c r="F8" s="38" t="s">
         <v>38</v>
       </c>
-      <c r="G8" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="H8" s="17">
+      <c r="G8" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="H8" s="39">
         <v>5.1681999999999999E-2</v>
       </c>
-      <c r="I8" s="28">
+      <c r="I8" s="34">
         <v>6.4625600000000005E-2</v>
       </c>
-      <c r="J8" s="17">
+      <c r="J8" s="39">
         <v>9</v>
       </c>
-      <c r="K8" s="29" t="s">
+      <c r="K8" s="40"/>
+      <c r="L8" s="24" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="45">
-      <c r="A9" s="19">
+    <row r="9" spans="1:12" ht="45">
+      <c r="A9" s="36">
         <v>6</v>
       </c>
-      <c r="B9" s="27" t="s">
+      <c r="B9" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="C9" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="25" t="s">
+      <c r="C9" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="E9" s="18" t="s">
+      <c r="E9" s="38" t="s">
         <v>38</v>
       </c>
-      <c r="F9" s="18" t="s">
+      <c r="F9" s="38" t="s">
         <v>38</v>
       </c>
-      <c r="G9" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="H9" s="21">
+      <c r="G9" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="H9" s="39">
         <v>5.1711E-2</v>
       </c>
-      <c r="I9" s="28">
+      <c r="I9" s="34">
         <v>6.4605700000000002E-2</v>
       </c>
-      <c r="J9" s="21">
+      <c r="J9" s="39">
         <v>11</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" ht="33.75">
-      <c r="A10" s="19">
+      <c r="K9" s="40"/>
+    </row>
+    <row r="10" spans="1:12" ht="45">
+      <c r="A10" s="36">
         <v>7</v>
       </c>
-      <c r="B10" s="27" t="s">
+      <c r="B10" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="C10" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10" s="25" t="s">
+      <c r="C10" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="E10" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="F10" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="G10" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="H10" s="21">
+      <c r="E10" s="38" t="s">
+        <v>51</v>
+      </c>
+      <c r="F10" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="G10" s="33" t="s">
+        <v>53</v>
+      </c>
+      <c r="H10" s="39">
         <v>5.1580000000000001E-2</v>
       </c>
-      <c r="I10" s="30">
+      <c r="I10" s="34">
         <v>6.4518699999999998E-2</v>
       </c>
-      <c r="J10" s="21">
+      <c r="J10" s="39">
         <v>12</v>
       </c>
-      <c r="K10" s="29" t="s">
+      <c r="K10" s="40"/>
+      <c r="L10" s="24" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
-      <c r="B11" s="22"/>
+    <row r="11" spans="1:12" ht="123.75">
+      <c r="A11" s="41">
+        <v>8</v>
+      </c>
+      <c r="B11" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="38" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="E11" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="H11" s="39">
+        <v>0.51668700000000001</v>
+      </c>
+      <c r="I11" s="43">
+        <v>6.4663100000000001E-2</v>
+      </c>
+      <c r="J11" s="39">
+        <v>15</v>
+      </c>
+      <c r="K11" s="40"/>
+    </row>
+    <row r="12" spans="1:12" ht="25.5">
+      <c r="A12" s="41">
+        <v>9</v>
+      </c>
+      <c r="B12" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="H12" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="I12" s="43">
+        <v>6.4527600000000004E-2</v>
+      </c>
+      <c r="J12" s="33">
+        <v>16</v>
+      </c>
+      <c r="K12" s="35"/>
+    </row>
+    <row r="13" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A13" s="45">
+        <v>10</v>
+      </c>
+      <c r="B13" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="47" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" s="47" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="H13" s="49">
+        <v>5.1580000000000001E-2</v>
+      </c>
+      <c r="I13" s="50">
+        <v>6.4497299999999994E-2</v>
+      </c>
+      <c r="J13" s="60">
+        <v>17</v>
+      </c>
+      <c r="K13" s="51"/>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="52"/>
+      <c r="B14" s="53"/>
+      <c r="C14" s="54" t="s">
+        <v>58</v>
+      </c>
+      <c r="D14" s="54" t="s">
+        <v>57</v>
+      </c>
+      <c r="E14" s="55"/>
+      <c r="F14" s="55"/>
+      <c r="G14" s="55"/>
+      <c r="H14" s="56">
+        <v>5.1648899999999998E-2</v>
+      </c>
+      <c r="I14" s="57"/>
+      <c r="J14" s="61"/>
+      <c r="K14" s="58"/>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" s="45">
+        <v>11</v>
+      </c>
+      <c r="B15" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="47" t="s">
+        <v>59</v>
+      </c>
+      <c r="D15" s="47" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="G15" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="H15" s="49">
+        <v>5.1717800000000001E-2</v>
+      </c>
+      <c r="I15" s="50">
+        <v>6.4495999999999998E-2</v>
+      </c>
+      <c r="J15" s="60">
+        <v>20</v>
+      </c>
+      <c r="K15" s="51"/>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" s="52"/>
+      <c r="B16" s="53"/>
+      <c r="C16" s="54" t="s">
+        <v>60</v>
+      </c>
+      <c r="D16" s="54" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" s="55"/>
+      <c r="F16" s="55"/>
+      <c r="G16" s="55"/>
+      <c r="H16" s="56">
+        <v>5.1648899999999998E-2</v>
+      </c>
+      <c r="I16" s="57"/>
+      <c r="J16" s="61"/>
+      <c r="K16" s="58"/>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17" s="45">
+        <v>12</v>
+      </c>
+      <c r="B17" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="47" t="s">
+        <v>61</v>
+      </c>
+      <c r="D17" s="47" t="s">
+        <v>23</v>
+      </c>
+      <c r="E17" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="F17" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="G17" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="H17" s="49">
+        <v>5.1855600000000002E-2</v>
+      </c>
+      <c r="I17" s="50">
+        <v>6.4500699999999994E-2</v>
+      </c>
+      <c r="J17" s="60">
+        <v>21</v>
+      </c>
+      <c r="K17" s="51"/>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18" s="52"/>
+      <c r="B18" s="53"/>
+      <c r="C18" s="54" t="s">
+        <v>62</v>
+      </c>
+      <c r="D18" s="54" t="s">
+        <v>23</v>
+      </c>
+      <c r="E18" s="55"/>
+      <c r="F18" s="55"/>
+      <c r="G18" s="55"/>
+      <c r="H18" s="56">
+        <v>5.1648899999999998E-2</v>
+      </c>
+      <c r="I18" s="57"/>
+      <c r="J18" s="61"/>
+      <c r="K18" s="58"/>
     </row>
   </sheetData>
+  <mergeCells count="24">
+    <mergeCell ref="I17:I18"/>
+    <mergeCell ref="K17:K18"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="J15:J16"/>
+    <mergeCell ref="J17:J18"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="G17:G18"/>
+    <mergeCell ref="K13:K14"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="I15:I16"/>
+    <mergeCell ref="K15:K16"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="I13:I14"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
+  <conditionalFormatting sqref="I1:J3 I19:J1048576 I4:I18">
+    <cfRule type="top10" dxfId="0" priority="1" bottom="1" rank="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1346,10 +1848,10 @@
       <c r="D10" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="31" t="s">
+      <c r="E10" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="F10" s="31"/>
+      <c r="F10" s="28"/>
       <c r="G10" s="14" t="s">
         <v>23</v>
       </c>

</xml_diff>

<commit_message>
* Changed num_boost_round and run again.
</commit_message>
<xml_diff>
--- a/training_result.xlsx
+++ b/training_result.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5355" yWindow="0" windowWidth="18690" windowHeight="11685"/>
+    <workbookView xWindow="6585" yWindow="0" windowWidth="18690" windowHeight="11685"/>
   </bookViews>
   <sheets>
     <sheet name="kernel_private" sheetId="6" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="70">
   <si>
     <t>Model</t>
   </si>
@@ -268,6 +268,27 @@
   </si>
   <si>
     <t>github version</t>
+  </si>
+  <si>
+    <t>lightgbm: 0</t>
+  </si>
+  <si>
+    <t>xgboost: 1.0</t>
+  </si>
+  <si>
+    <t>0.051647/1770</t>
+  </si>
+  <si>
+    <t>+ eta: 0.006
++ max_depth: 6
++ child_weight: 2
++ subsample: 0.4
++ bytree: 0.4
++ lambda: 8.0
++ alpha: 0.8</t>
+  </si>
+  <si>
+    <t>0.050215/5000</t>
   </si>
 </sst>
 </file>
@@ -495,7 +516,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -578,9 +599,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -629,55 +647,61 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -695,7 +719,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF0070C0"/>
+          <bgColor rgb="FF00B0F0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -994,11 +1018,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L18"/>
+  <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
+      <pane ySplit="3" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1073,7 +1097,7 @@
       <c r="I3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="J3" s="59" t="s">
+      <c r="J3" s="48" t="s">
         <v>63</v>
       </c>
       <c r="K3" s="5" t="s">
@@ -1081,37 +1105,37 @@
       </c>
     </row>
     <row r="4" spans="1:12" s="19" customFormat="1" ht="78.75">
-      <c r="A4" s="29">
+      <c r="A4" s="28">
         <v>1</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="31" t="s">
+      <c r="C4" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="30" t="s">
+      <c r="D4" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="32" t="s">
+      <c r="E4" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="F4" s="33" t="s">
+      <c r="F4" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="G4" s="33" t="s">
+      <c r="G4" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="H4" s="33">
+      <c r="H4" s="32">
         <v>5.1650000000000001E-2</v>
       </c>
-      <c r="I4" s="34">
+      <c r="I4" s="33">
         <v>6.4611000000000002E-2</v>
       </c>
-      <c r="J4" s="33">
+      <c r="J4" s="32">
         <v>2</v>
       </c>
-      <c r="K4" s="35"/>
+      <c r="K4" s="34"/>
     </row>
     <row r="5" spans="1:12" s="19" customFormat="1" ht="33.75">
       <c r="A5" s="19">
@@ -1138,437 +1162,541 @@
       <c r="H5" s="18">
         <v>5.1652999999999998E-2</v>
       </c>
-      <c r="I5" s="34">
+      <c r="I5" s="33">
         <v>6.4565600000000001E-2</v>
       </c>
-      <c r="J5" s="33">
+      <c r="J5" s="32">
         <v>3</v>
       </c>
-      <c r="K5" s="35"/>
+      <c r="K5" s="34"/>
     </row>
     <row r="6" spans="1:12" ht="67.5">
-      <c r="A6" s="36">
+      <c r="A6" s="35">
         <v>3</v>
       </c>
-      <c r="B6" s="37" t="s">
+      <c r="B6" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="C6" s="38" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="30" t="s">
+      <c r="C6" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="E6" s="38" t="s">
+      <c r="E6" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="F6" s="38" t="s">
+      <c r="F6" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="G6" s="38" t="s">
-        <v>23</v>
-      </c>
-      <c r="H6" s="38">
+      <c r="G6" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6" s="37">
         <v>5.1644000000000002E-2</v>
       </c>
-      <c r="I6" s="34">
+      <c r="I6" s="33">
         <v>6.4564800000000006E-2</v>
       </c>
-      <c r="J6" s="33">
+      <c r="J6" s="32">
         <v>7</v>
       </c>
-      <c r="K6" s="35"/>
+      <c r="K6" s="34"/>
     </row>
     <row r="7" spans="1:12" ht="33.75">
-      <c r="A7" s="36">
+      <c r="A7" s="35">
         <v>4</v>
       </c>
-      <c r="B7" s="37" t="s">
+      <c r="B7" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="C7" s="38" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="30" t="s">
+      <c r="C7" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="E7" s="38" t="s">
+      <c r="E7" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="F7" s="38" t="s">
+      <c r="F7" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="G7" s="38" t="s">
-        <v>23</v>
-      </c>
-      <c r="H7" s="38">
+      <c r="G7" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7" s="37">
         <v>5.1604999999999998E-2</v>
       </c>
-      <c r="I7" s="34">
+      <c r="I7" s="33">
         <v>6.4559000000000005E-2</v>
       </c>
-      <c r="J7" s="33">
+      <c r="J7" s="32">
         <v>8</v>
       </c>
-      <c r="K7" s="35"/>
+      <c r="K7" s="34"/>
     </row>
     <row r="8" spans="1:12" ht="33.75">
-      <c r="A8" s="36">
+      <c r="A8" s="35">
         <v>5</v>
       </c>
-      <c r="B8" s="37" t="s">
+      <c r="B8" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="38" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="30" t="s">
+      <c r="C8" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="E8" s="38" t="s">
+      <c r="E8" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="F8" s="38" t="s">
+      <c r="F8" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="G8" s="38" t="s">
-        <v>23</v>
-      </c>
-      <c r="H8" s="39">
+      <c r="G8" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="H8" s="38">
         <v>5.1681999999999999E-2</v>
       </c>
-      <c r="I8" s="34">
+      <c r="I8" s="33">
         <v>6.4625600000000005E-2</v>
       </c>
-      <c r="J8" s="39">
+      <c r="J8" s="38">
         <v>9</v>
       </c>
-      <c r="K8" s="40"/>
+      <c r="K8" s="39"/>
       <c r="L8" s="24" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="45">
-      <c r="A9" s="36">
+      <c r="A9" s="35">
         <v>6</v>
       </c>
-      <c r="B9" s="37" t="s">
+      <c r="B9" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="C9" s="38" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="30" t="s">
+      <c r="C9" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="E9" s="38" t="s">
+      <c r="E9" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="F9" s="38" t="s">
+      <c r="F9" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="G9" s="38" t="s">
-        <v>23</v>
-      </c>
-      <c r="H9" s="39">
+      <c r="G9" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="H9" s="38">
         <v>5.1711E-2</v>
       </c>
-      <c r="I9" s="34">
+      <c r="I9" s="33">
         <v>6.4605700000000002E-2</v>
       </c>
-      <c r="J9" s="39">
+      <c r="J9" s="38">
         <v>11</v>
       </c>
-      <c r="K9" s="40"/>
+      <c r="K9" s="39"/>
     </row>
     <row r="10" spans="1:12" ht="45">
-      <c r="A10" s="36">
+      <c r="A10" s="35">
         <v>7</v>
       </c>
-      <c r="B10" s="37" t="s">
+      <c r="B10" s="36" t="s">
         <v>47</v>
       </c>
-      <c r="C10" s="38" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10" s="30" t="s">
+      <c r="C10" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="E10" s="38" t="s">
+      <c r="E10" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="F10" s="38" t="s">
+      <c r="F10" s="37" t="s">
         <v>52</v>
       </c>
-      <c r="G10" s="33" t="s">
+      <c r="G10" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="H10" s="39">
+      <c r="H10" s="38">
         <v>5.1580000000000001E-2</v>
       </c>
-      <c r="I10" s="34">
+      <c r="I10" s="33">
         <v>6.4518699999999998E-2</v>
       </c>
-      <c r="J10" s="39">
+      <c r="J10" s="38">
         <v>12</v>
       </c>
-      <c r="K10" s="40"/>
+      <c r="K10" s="39"/>
       <c r="L10" s="24" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="123.75">
-      <c r="A11" s="41">
+      <c r="A11" s="40">
         <v>8</v>
       </c>
-      <c r="B11" s="42" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="38" t="s">
+      <c r="B11" s="41" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="37" t="s">
         <v>49</v>
       </c>
-      <c r="D11" s="30" t="s">
+      <c r="D11" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="E11" s="38" t="s">
-        <v>23</v>
-      </c>
-      <c r="F11" s="38" t="s">
-        <v>23</v>
-      </c>
-      <c r="G11" s="38" t="s">
-        <v>23</v>
-      </c>
-      <c r="H11" s="39">
+      <c r="E11" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="H11" s="38">
         <v>0.51668700000000001</v>
       </c>
-      <c r="I11" s="43">
+      <c r="I11" s="42">
         <v>6.4663100000000001E-2</v>
       </c>
-      <c r="J11" s="39">
+      <c r="J11" s="38">
         <v>15</v>
       </c>
-      <c r="K11" s="40"/>
+      <c r="K11" s="39"/>
     </row>
     <row r="12" spans="1:12" ht="25.5">
-      <c r="A12" s="41">
+      <c r="A12" s="40">
         <v>9</v>
       </c>
-      <c r="B12" s="44" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" s="44" t="s">
+      <c r="B12" s="43" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="43" t="s">
         <v>54</v>
       </c>
-      <c r="D12" s="44" t="s">
-        <v>23</v>
-      </c>
-      <c r="E12" s="38" t="s">
-        <v>23</v>
-      </c>
-      <c r="F12" s="38" t="s">
-        <v>23</v>
-      </c>
-      <c r="G12" s="38" t="s">
-        <v>23</v>
-      </c>
-      <c r="H12" s="38" t="s">
+      <c r="D12" s="43" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="H12" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="I12" s="43">
+      <c r="I12" s="42">
         <v>6.4527600000000004E-2</v>
       </c>
-      <c r="J12" s="33">
+      <c r="J12" s="32">
         <v>16</v>
       </c>
-      <c r="K12" s="35"/>
+      <c r="K12" s="34"/>
     </row>
     <row r="13" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A13" s="45">
+      <c r="A13" s="56">
         <v>10</v>
       </c>
-      <c r="B13" s="46" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13" s="47" t="s">
+      <c r="B13" s="58" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="44" t="s">
         <v>56</v>
       </c>
-      <c r="D13" s="47" t="s">
-        <v>23</v>
-      </c>
-      <c r="E13" s="48" t="s">
-        <v>23</v>
-      </c>
-      <c r="F13" s="48" t="s">
-        <v>23</v>
-      </c>
-      <c r="G13" s="48" t="s">
-        <v>23</v>
-      </c>
-      <c r="H13" s="49">
+      <c r="D13" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="60" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="60" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13" s="60" t="s">
+        <v>23</v>
+      </c>
+      <c r="H13" s="45">
         <v>5.1580000000000001E-2</v>
       </c>
       <c r="I13" s="50">
         <v>6.4497299999999994E-2</v>
       </c>
-      <c r="J13" s="60">
+      <c r="J13" s="54">
         <v>17</v>
       </c>
-      <c r="K13" s="51"/>
+      <c r="K13" s="52"/>
     </row>
     <row r="14" spans="1:12">
-      <c r="A14" s="52"/>
-      <c r="B14" s="53"/>
-      <c r="C14" s="54" t="s">
+      <c r="A14" s="57"/>
+      <c r="B14" s="59"/>
+      <c r="C14" s="46" t="s">
         <v>58</v>
       </c>
-      <c r="D14" s="54" t="s">
+      <c r="D14" s="46" t="s">
         <v>57</v>
       </c>
-      <c r="E14" s="55"/>
-      <c r="F14" s="55"/>
-      <c r="G14" s="55"/>
-      <c r="H14" s="56">
+      <c r="E14" s="61"/>
+      <c r="F14" s="61"/>
+      <c r="G14" s="61"/>
+      <c r="H14" s="47">
         <v>5.1648899999999998E-2</v>
       </c>
-      <c r="I14" s="57"/>
-      <c r="J14" s="61"/>
-      <c r="K14" s="58"/>
+      <c r="I14" s="51"/>
+      <c r="J14" s="55"/>
+      <c r="K14" s="53"/>
     </row>
     <row r="15" spans="1:12">
-      <c r="A15" s="45">
+      <c r="A15" s="56">
         <v>11</v>
       </c>
-      <c r="B15" s="46" t="s">
-        <v>23</v>
-      </c>
-      <c r="C15" s="47" t="s">
+      <c r="B15" s="58" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="44" t="s">
         <v>59</v>
       </c>
-      <c r="D15" s="47" t="s">
-        <v>23</v>
-      </c>
-      <c r="E15" s="48" t="s">
-        <v>23</v>
-      </c>
-      <c r="F15" s="48" t="s">
-        <v>23</v>
-      </c>
-      <c r="G15" s="48" t="s">
-        <v>23</v>
-      </c>
-      <c r="H15" s="49">
+      <c r="D15" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" s="60" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15" s="60" t="s">
+        <v>23</v>
+      </c>
+      <c r="G15" s="60" t="s">
+        <v>23</v>
+      </c>
+      <c r="H15" s="45">
         <v>5.1717800000000001E-2</v>
       </c>
       <c r="I15" s="50">
         <v>6.4495999999999998E-2</v>
       </c>
-      <c r="J15" s="60">
+      <c r="J15" s="54">
         <v>20</v>
       </c>
-      <c r="K15" s="51"/>
+      <c r="K15" s="52"/>
     </row>
     <row r="16" spans="1:12">
-      <c r="A16" s="52"/>
-      <c r="B16" s="53"/>
-      <c r="C16" s="54" t="s">
+      <c r="A16" s="57"/>
+      <c r="B16" s="59"/>
+      <c r="C16" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="D16" s="54" t="s">
-        <v>23</v>
-      </c>
-      <c r="E16" s="55"/>
-      <c r="F16" s="55"/>
-      <c r="G16" s="55"/>
-      <c r="H16" s="56">
+      <c r="D16" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" s="61"/>
+      <c r="F16" s="61"/>
+      <c r="G16" s="61"/>
+      <c r="H16" s="47">
         <v>5.1648899999999998E-2</v>
       </c>
-      <c r="I16" s="57"/>
-      <c r="J16" s="61"/>
-      <c r="K16" s="58"/>
+      <c r="I16" s="51"/>
+      <c r="J16" s="55"/>
+      <c r="K16" s="53"/>
     </row>
     <row r="17" spans="1:11">
-      <c r="A17" s="45">
+      <c r="A17" s="56">
         <v>12</v>
       </c>
-      <c r="B17" s="46" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" s="47" t="s">
+      <c r="B17" s="58" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="44" t="s">
         <v>61</v>
       </c>
-      <c r="D17" s="47" t="s">
-        <v>23</v>
-      </c>
-      <c r="E17" s="48" t="s">
-        <v>23</v>
-      </c>
-      <c r="F17" s="48" t="s">
-        <v>23</v>
-      </c>
-      <c r="G17" s="48" t="s">
-        <v>23</v>
-      </c>
-      <c r="H17" s="49">
+      <c r="D17" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="E17" s="60" t="s">
+        <v>23</v>
+      </c>
+      <c r="F17" s="60" t="s">
+        <v>23</v>
+      </c>
+      <c r="G17" s="60" t="s">
+        <v>23</v>
+      </c>
+      <c r="H17" s="45">
         <v>5.1855600000000002E-2</v>
       </c>
       <c r="I17" s="50">
         <v>6.4500699999999994E-2</v>
       </c>
-      <c r="J17" s="60">
+      <c r="J17" s="54">
         <v>21</v>
       </c>
-      <c r="K17" s="51"/>
+      <c r="K17" s="52"/>
     </row>
     <row r="18" spans="1:11">
-      <c r="A18" s="52"/>
-      <c r="B18" s="53"/>
-      <c r="C18" s="54" t="s">
+      <c r="A18" s="57"/>
+      <c r="B18" s="59"/>
+      <c r="C18" s="46" t="s">
         <v>62</v>
       </c>
-      <c r="D18" s="54" t="s">
-        <v>23</v>
-      </c>
-      <c r="E18" s="55"/>
-      <c r="F18" s="55"/>
-      <c r="G18" s="55"/>
-      <c r="H18" s="56">
+      <c r="D18" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="E18" s="61"/>
+      <c r="F18" s="61"/>
+      <c r="G18" s="61"/>
+      <c r="H18" s="47">
         <v>5.1648899999999998E-2</v>
       </c>
-      <c r="I18" s="57"/>
-      <c r="J18" s="61"/>
-      <c r="K18" s="58"/>
+      <c r="I18" s="51"/>
+      <c r="J18" s="55"/>
+      <c r="K18" s="53"/>
+    </row>
+    <row r="19" spans="1:11" ht="78.75">
+      <c r="B19" s="58" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="44" t="s">
+        <v>66</v>
+      </c>
+      <c r="D19" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="E19" s="60" t="s">
+        <v>23</v>
+      </c>
+      <c r="F19" s="60" t="s">
+        <v>23</v>
+      </c>
+      <c r="G19" s="60" t="s">
+        <v>23</v>
+      </c>
+      <c r="H19" s="45" t="s">
+        <v>67</v>
+      </c>
+      <c r="I19" s="50">
+        <v>6.4522999999999997E-2</v>
+      </c>
+      <c r="J19" s="54"/>
+      <c r="K19" s="52">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="B20" s="59"/>
+      <c r="C20" s="46" t="s">
+        <v>65</v>
+      </c>
+      <c r="D20" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="E20" s="61"/>
+      <c r="F20" s="61"/>
+      <c r="G20" s="61"/>
+      <c r="H20" s="49"/>
+      <c r="I20" s="51"/>
+      <c r="J20" s="55"/>
+      <c r="K20" s="53"/>
+    </row>
+    <row r="21" spans="1:11" ht="25.5">
+      <c r="B21" s="58" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" s="44" t="s">
+        <v>66</v>
+      </c>
+      <c r="D21" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="E21" s="60" t="s">
+        <v>23</v>
+      </c>
+      <c r="F21" s="60" t="s">
+        <v>23</v>
+      </c>
+      <c r="G21" s="60" t="s">
+        <v>23</v>
+      </c>
+      <c r="H21" s="45" t="s">
+        <v>69</v>
+      </c>
+      <c r="I21" s="50"/>
+      <c r="J21" s="54"/>
+      <c r="K21" s="52">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="B22" s="59"/>
+      <c r="C22" s="46" t="s">
+        <v>65</v>
+      </c>
+      <c r="D22" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="E22" s="61"/>
+      <c r="F22" s="61"/>
+      <c r="G22" s="61"/>
+      <c r="H22" s="49"/>
+      <c r="I22" s="51"/>
+      <c r="J22" s="55"/>
+      <c r="K22" s="53"/>
     </row>
   </sheetData>
-  <mergeCells count="24">
+  <mergeCells count="38">
+    <mergeCell ref="J19:J20"/>
+    <mergeCell ref="K19:K20"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="G21:G22"/>
+    <mergeCell ref="I21:I22"/>
+    <mergeCell ref="J21:J22"/>
+    <mergeCell ref="K21:K22"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="I19:I20"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="G17:G18"/>
     <mergeCell ref="I17:I18"/>
     <mergeCell ref="K17:K18"/>
     <mergeCell ref="J13:J14"/>
     <mergeCell ref="J15:J16"/>
     <mergeCell ref="J17:J18"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="G17:G18"/>
     <mergeCell ref="K13:K14"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="G15:G16"/>
     <mergeCell ref="I15:I16"/>
     <mergeCell ref="K15:K16"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="G13:G14"/>
     <mergeCell ref="I13:I14"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="I1:J3 I19:J1048576 I4:I18">
-    <cfRule type="top10" dxfId="0" priority="1" bottom="1" rank="1"/>
+  <conditionalFormatting sqref="I1:J3 I23:J1048576 I4:I22">
+    <cfRule type="top10" dxfId="2" priority="1" bottom="1" rank="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1848,10 +1976,10 @@
       <c r="D10" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="28" t="s">
+      <c r="E10" s="62" t="s">
         <v>26</v>
       </c>
-      <c r="F10" s="28"/>
+      <c r="F10" s="62"/>
       <c r="G10" s="14" t="s">
         <v>23</v>
       </c>

</xml_diff>

<commit_message>
* Added training data 2016 and 2017. * Updated training result.
</commit_message>
<xml_diff>
--- a/training_result.xlsx
+++ b/training_result.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6585" yWindow="0" windowWidth="18690" windowHeight="11685"/>
+    <workbookView xWindow="7815" yWindow="0" windowWidth="18690" windowHeight="11685"/>
   </bookViews>
   <sheets>
     <sheet name="kernel_private" sheetId="6" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="69">
   <si>
     <t>Model</t>
   </si>
@@ -286,9 +286,6 @@
 + bytree: 0.4
 + lambda: 8.0
 + alpha: 0.8</t>
-  </si>
-  <si>
-    <t>0.050215/5000</t>
   </si>
 </sst>
 </file>
@@ -665,40 +662,40 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -708,21 +705,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill>
@@ -1022,7 +1005,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H22" sqref="H22"/>
+      <selection pane="bottomLeft" activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1408,10 +1391,10 @@
       <c r="K12" s="34"/>
     </row>
     <row r="13" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A13" s="56">
+      <c r="A13" s="60">
         <v>10</v>
       </c>
-      <c r="B13" s="58" t="s">
+      <c r="B13" s="54" t="s">
         <v>23</v>
       </c>
       <c r="C13" s="44" t="s">
@@ -1420,50 +1403,50 @@
       <c r="D13" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="E13" s="60" t="s">
-        <v>23</v>
-      </c>
-      <c r="F13" s="60" t="s">
-        <v>23</v>
-      </c>
-      <c r="G13" s="60" t="s">
+      <c r="E13" s="56" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="56" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13" s="56" t="s">
         <v>23</v>
       </c>
       <c r="H13" s="45">
         <v>5.1580000000000001E-2</v>
       </c>
-      <c r="I13" s="50">
+      <c r="I13" s="58">
         <v>6.4497299999999994E-2</v>
       </c>
-      <c r="J13" s="54">
+      <c r="J13" s="50">
         <v>17</v>
       </c>
       <c r="K13" s="52"/>
     </row>
     <row r="14" spans="1:12">
-      <c r="A14" s="57"/>
-      <c r="B14" s="59"/>
+      <c r="A14" s="61"/>
+      <c r="B14" s="55"/>
       <c r="C14" s="46" t="s">
         <v>58</v>
       </c>
       <c r="D14" s="46" t="s">
         <v>57</v>
       </c>
-      <c r="E14" s="61"/>
-      <c r="F14" s="61"/>
-      <c r="G14" s="61"/>
+      <c r="E14" s="57"/>
+      <c r="F14" s="57"/>
+      <c r="G14" s="57"/>
       <c r="H14" s="47">
         <v>5.1648899999999998E-2</v>
       </c>
-      <c r="I14" s="51"/>
-      <c r="J14" s="55"/>
+      <c r="I14" s="59"/>
+      <c r="J14" s="51"/>
       <c r="K14" s="53"/>
     </row>
     <row r="15" spans="1:12">
-      <c r="A15" s="56">
+      <c r="A15" s="60">
         <v>11</v>
       </c>
-      <c r="B15" s="58" t="s">
+      <c r="B15" s="54" t="s">
         <v>23</v>
       </c>
       <c r="C15" s="44" t="s">
@@ -1472,50 +1455,50 @@
       <c r="D15" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="E15" s="60" t="s">
-        <v>23</v>
-      </c>
-      <c r="F15" s="60" t="s">
-        <v>23</v>
-      </c>
-      <c r="G15" s="60" t="s">
+      <c r="E15" s="56" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15" s="56" t="s">
+        <v>23</v>
+      </c>
+      <c r="G15" s="56" t="s">
         <v>23</v>
       </c>
       <c r="H15" s="45">
         <v>5.1717800000000001E-2</v>
       </c>
-      <c r="I15" s="50">
+      <c r="I15" s="58">
         <v>6.4495999999999998E-2</v>
       </c>
-      <c r="J15" s="54">
+      <c r="J15" s="50">
         <v>20</v>
       </c>
       <c r="K15" s="52"/>
     </row>
     <row r="16" spans="1:12">
-      <c r="A16" s="57"/>
-      <c r="B16" s="59"/>
+      <c r="A16" s="61"/>
+      <c r="B16" s="55"/>
       <c r="C16" s="46" t="s">
         <v>60</v>
       </c>
       <c r="D16" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="E16" s="61"/>
-      <c r="F16" s="61"/>
-      <c r="G16" s="61"/>
+      <c r="E16" s="57"/>
+      <c r="F16" s="57"/>
+      <c r="G16" s="57"/>
       <c r="H16" s="47">
         <v>5.1648899999999998E-2</v>
       </c>
-      <c r="I16" s="51"/>
-      <c r="J16" s="55"/>
+      <c r="I16" s="59"/>
+      <c r="J16" s="51"/>
       <c r="K16" s="53"/>
     </row>
     <row r="17" spans="1:11">
-      <c r="A17" s="56">
+      <c r="A17" s="60">
         <v>12</v>
       </c>
-      <c r="B17" s="58" t="s">
+      <c r="B17" s="54" t="s">
         <v>23</v>
       </c>
       <c r="C17" s="44" t="s">
@@ -1524,47 +1507,47 @@
       <c r="D17" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="E17" s="60" t="s">
-        <v>23</v>
-      </c>
-      <c r="F17" s="60" t="s">
-        <v>23</v>
-      </c>
-      <c r="G17" s="60" t="s">
+      <c r="E17" s="56" t="s">
+        <v>23</v>
+      </c>
+      <c r="F17" s="56" t="s">
+        <v>23</v>
+      </c>
+      <c r="G17" s="56" t="s">
         <v>23</v>
       </c>
       <c r="H17" s="45">
         <v>5.1855600000000002E-2</v>
       </c>
-      <c r="I17" s="50">
+      <c r="I17" s="58">
         <v>6.4500699999999994E-2</v>
       </c>
-      <c r="J17" s="54">
+      <c r="J17" s="50">
         <v>21</v>
       </c>
       <c r="K17" s="52"/>
     </row>
     <row r="18" spans="1:11">
-      <c r="A18" s="57"/>
-      <c r="B18" s="59"/>
+      <c r="A18" s="61"/>
+      <c r="B18" s="55"/>
       <c r="C18" s="46" t="s">
         <v>62</v>
       </c>
       <c r="D18" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="E18" s="61"/>
-      <c r="F18" s="61"/>
-      <c r="G18" s="61"/>
+      <c r="E18" s="57"/>
+      <c r="F18" s="57"/>
+      <c r="G18" s="57"/>
       <c r="H18" s="47">
         <v>5.1648899999999998E-2</v>
       </c>
-      <c r="I18" s="51"/>
-      <c r="J18" s="55"/>
+      <c r="I18" s="59"/>
+      <c r="J18" s="51"/>
       <c r="K18" s="53"/>
     </row>
     <row r="19" spans="1:11" ht="78.75">
-      <c r="B19" s="58" t="s">
+      <c r="B19" s="54" t="s">
         <v>23</v>
       </c>
       <c r="C19" s="44" t="s">
@@ -1573,44 +1556,44 @@
       <c r="D19" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="E19" s="60" t="s">
-        <v>23</v>
-      </c>
-      <c r="F19" s="60" t="s">
-        <v>23</v>
-      </c>
-      <c r="G19" s="60" t="s">
+      <c r="E19" s="56" t="s">
+        <v>23</v>
+      </c>
+      <c r="F19" s="56" t="s">
+        <v>23</v>
+      </c>
+      <c r="G19" s="56" t="s">
         <v>23</v>
       </c>
       <c r="H19" s="45" t="s">
         <v>67</v>
       </c>
-      <c r="I19" s="50">
+      <c r="I19" s="58">
         <v>6.4522999999999997E-2</v>
       </c>
-      <c r="J19" s="54"/>
+      <c r="J19" s="50"/>
       <c r="K19" s="52">
         <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:11">
-      <c r="B20" s="59"/>
+      <c r="B20" s="55"/>
       <c r="C20" s="46" t="s">
         <v>65</v>
       </c>
       <c r="D20" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="E20" s="61"/>
-      <c r="F20" s="61"/>
-      <c r="G20" s="61"/>
+      <c r="E20" s="57"/>
+      <c r="F20" s="57"/>
+      <c r="G20" s="57"/>
       <c r="H20" s="49"/>
-      <c r="I20" s="51"/>
-      <c r="J20" s="55"/>
+      <c r="I20" s="59"/>
+      <c r="J20" s="51"/>
       <c r="K20" s="53"/>
     </row>
-    <row r="21" spans="1:11" ht="25.5">
-      <c r="B21" s="58" t="s">
+    <row r="21" spans="1:11">
+      <c r="B21" s="54" t="s">
         <v>23</v>
       </c>
       <c r="C21" s="44" t="s">
@@ -1619,42 +1602,62 @@
       <c r="D21" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="E21" s="60" t="s">
-        <v>23</v>
-      </c>
-      <c r="F21" s="60" t="s">
-        <v>23</v>
-      </c>
-      <c r="G21" s="60" t="s">
-        <v>23</v>
-      </c>
-      <c r="H21" s="45" t="s">
-        <v>69</v>
-      </c>
-      <c r="I21" s="50"/>
-      <c r="J21" s="54"/>
-      <c r="K21" s="52">
-        <v>12</v>
-      </c>
+      <c r="E21" s="56" t="s">
+        <v>23</v>
+      </c>
+      <c r="F21" s="56" t="s">
+        <v>23</v>
+      </c>
+      <c r="G21" s="56" t="s">
+        <v>23</v>
+      </c>
+      <c r="H21" s="45"/>
+      <c r="I21" s="58"/>
+      <c r="J21" s="50"/>
+      <c r="K21" s="52"/>
     </row>
     <row r="22" spans="1:11">
-      <c r="B22" s="59"/>
+      <c r="B22" s="55"/>
       <c r="C22" s="46" t="s">
         <v>65</v>
       </c>
       <c r="D22" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="E22" s="61"/>
-      <c r="F22" s="61"/>
-      <c r="G22" s="61"/>
+      <c r="E22" s="57"/>
+      <c r="F22" s="57"/>
+      <c r="G22" s="57"/>
       <c r="H22" s="49"/>
-      <c r="I22" s="51"/>
-      <c r="J22" s="55"/>
+      <c r="I22" s="59"/>
+      <c r="J22" s="51"/>
       <c r="K22" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="I17:I18"/>
+    <mergeCell ref="K17:K18"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="J15:J16"/>
+    <mergeCell ref="J17:J18"/>
+    <mergeCell ref="K13:K14"/>
+    <mergeCell ref="I15:I16"/>
+    <mergeCell ref="K15:K16"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="G17:G18"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="G13:G14"/>
     <mergeCell ref="J19:J20"/>
     <mergeCell ref="K19:K20"/>
     <mergeCell ref="B21:B22"/>
@@ -1669,34 +1672,10 @@
     <mergeCell ref="F19:F20"/>
     <mergeCell ref="G19:G20"/>
     <mergeCell ref="I19:I20"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="G17:G18"/>
-    <mergeCell ref="I17:I18"/>
-    <mergeCell ref="K17:K18"/>
-    <mergeCell ref="J13:J14"/>
-    <mergeCell ref="J15:J16"/>
-    <mergeCell ref="J17:J18"/>
-    <mergeCell ref="K13:K14"/>
-    <mergeCell ref="I15:I16"/>
-    <mergeCell ref="K15:K16"/>
-    <mergeCell ref="I13:I14"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="I1:J3 I23:J1048576 I4:I22">
-    <cfRule type="top10" dxfId="2" priority="1" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="0" priority="1" bottom="1" rank="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
* Updated training result.
</commit_message>
<xml_diff>
--- a/training_result.xlsx
+++ b/training_result.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7815" yWindow="0" windowWidth="18690" windowHeight="11685"/>
+    <workbookView xWindow="9045" yWindow="0" windowWidth="18690" windowHeight="11685"/>
   </bookViews>
   <sheets>
     <sheet name="kernel_private" sheetId="6" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="72">
   <si>
     <t>Model</t>
   </si>
@@ -206,9 +206,6 @@
 + add fts: N-zip_count, N-city_count, N-GarPoolAC, mean_area, med_year, med_lat, med_long
 + remove fts: regionidcounty, poolsizesum, yardbuildingsqft26, decktypeid, storytypeid, pooltypeid2</t>
     <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>kernel name: xgboost version 2</t>
   </si>
   <si>
     <t>lightgbm</t>
@@ -286,6 +283,18 @@
 + bytree: 0.4
 + lambda: 8.0
 + alpha: 0.8</t>
+  </si>
+  <si>
+    <t>161371,58</t>
+  </si>
+  <si>
+    <t>0.05083/4990</t>
+  </si>
+  <si>
+    <t>prop 2016</t>
+  </si>
+  <si>
+    <t>kernel name: xgboost, lightgbm, combined models</t>
   </si>
 </sst>
 </file>
@@ -513,7 +522,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -662,16 +671,28 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -686,20 +707,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1004,8 +1016,8 @@
   <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K25" sqref="K25"/>
+      <pane ySplit="3" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1027,7 +1039,7 @@
     <row r="1" spans="1:12" s="22" customFormat="1" ht="27.75" customHeight="1">
       <c r="A1" s="21"/>
       <c r="B1" s="25" t="s">
-        <v>48</v>
+        <v>71</v>
       </c>
       <c r="C1" s="21"/>
       <c r="D1" s="21"/>
@@ -1081,10 +1093,10 @@
         <v>15</v>
       </c>
       <c r="J3" s="48" t="s">
+        <v>62</v>
+      </c>
+      <c r="K3" s="5" t="s">
         <v>63</v>
-      </c>
-      <c r="K3" s="5" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:12" s="19" customFormat="1" ht="78.75">
@@ -1302,13 +1314,13 @@
         <v>38</v>
       </c>
       <c r="E10" s="37" t="s">
+        <v>50</v>
+      </c>
+      <c r="F10" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="F10" s="37" t="s">
+      <c r="G10" s="32" t="s">
         <v>52</v>
-      </c>
-      <c r="G10" s="32" t="s">
-        <v>53</v>
       </c>
       <c r="H10" s="38">
         <v>5.1580000000000001E-2</v>
@@ -1332,10 +1344,10 @@
         <v>23</v>
       </c>
       <c r="C11" s="37" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11" s="29" t="s">
         <v>49</v>
-      </c>
-      <c r="D11" s="29" t="s">
-        <v>50</v>
       </c>
       <c r="E11" s="37" t="s">
         <v>23</v>
@@ -1365,22 +1377,22 @@
         <v>23</v>
       </c>
       <c r="C12" s="43" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" s="43" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="H12" s="37" t="s">
         <v>54</v>
-      </c>
-      <c r="D12" s="43" t="s">
-        <v>23</v>
-      </c>
-      <c r="E12" s="37" t="s">
-        <v>23</v>
-      </c>
-      <c r="F12" s="37" t="s">
-        <v>23</v>
-      </c>
-      <c r="G12" s="37" t="s">
-        <v>23</v>
-      </c>
-      <c r="H12" s="37" t="s">
-        <v>55</v>
       </c>
       <c r="I12" s="42">
         <v>6.4527600000000004E-2</v>
@@ -1391,273 +1403,255 @@
       <c r="K12" s="34"/>
     </row>
     <row r="13" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A13" s="60">
+      <c r="A13" s="56">
         <v>10</v>
       </c>
-      <c r="B13" s="54" t="s">
+      <c r="B13" s="58" t="s">
         <v>23</v>
       </c>
       <c r="C13" s="44" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D13" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="E13" s="56" t="s">
-        <v>23</v>
-      </c>
-      <c r="F13" s="56" t="s">
-        <v>23</v>
-      </c>
-      <c r="G13" s="56" t="s">
+      <c r="E13" s="60" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="60" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13" s="60" t="s">
         <v>23</v>
       </c>
       <c r="H13" s="45">
         <v>5.1580000000000001E-2</v>
       </c>
-      <c r="I13" s="58">
+      <c r="I13" s="50">
         <v>6.4497299999999994E-2</v>
       </c>
-      <c r="J13" s="50">
+      <c r="J13" s="54">
         <v>17</v>
       </c>
       <c r="K13" s="52"/>
     </row>
     <row r="14" spans="1:12">
-      <c r="A14" s="61"/>
-      <c r="B14" s="55"/>
+      <c r="A14" s="57"/>
+      <c r="B14" s="59"/>
       <c r="C14" s="46" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D14" s="46" t="s">
-        <v>57</v>
-      </c>
-      <c r="E14" s="57"/>
-      <c r="F14" s="57"/>
-      <c r="G14" s="57"/>
+        <v>56</v>
+      </c>
+      <c r="E14" s="61"/>
+      <c r="F14" s="61"/>
+      <c r="G14" s="61"/>
       <c r="H14" s="47">
         <v>5.1648899999999998E-2</v>
       </c>
-      <c r="I14" s="59"/>
-      <c r="J14" s="51"/>
+      <c r="I14" s="51"/>
+      <c r="J14" s="55"/>
       <c r="K14" s="53"/>
     </row>
     <row r="15" spans="1:12">
-      <c r="A15" s="60">
+      <c r="A15" s="56">
         <v>11</v>
       </c>
-      <c r="B15" s="54" t="s">
+      <c r="B15" s="58" t="s">
         <v>23</v>
       </c>
       <c r="C15" s="44" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D15" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="E15" s="56" t="s">
-        <v>23</v>
-      </c>
-      <c r="F15" s="56" t="s">
-        <v>23</v>
-      </c>
-      <c r="G15" s="56" t="s">
+      <c r="E15" s="60" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15" s="60" t="s">
+        <v>23</v>
+      </c>
+      <c r="G15" s="60" t="s">
         <v>23</v>
       </c>
       <c r="H15" s="45">
         <v>5.1717800000000001E-2</v>
       </c>
-      <c r="I15" s="58">
+      <c r="I15" s="50">
         <v>6.4495999999999998E-2</v>
       </c>
-      <c r="J15" s="50">
+      <c r="J15" s="54">
         <v>20</v>
       </c>
       <c r="K15" s="52"/>
     </row>
     <row r="16" spans="1:12">
-      <c r="A16" s="61"/>
-      <c r="B16" s="55"/>
+      <c r="A16" s="57"/>
+      <c r="B16" s="59"/>
       <c r="C16" s="46" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D16" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="E16" s="57"/>
-      <c r="F16" s="57"/>
-      <c r="G16" s="57"/>
+      <c r="E16" s="61"/>
+      <c r="F16" s="61"/>
+      <c r="G16" s="61"/>
       <c r="H16" s="47">
         <v>5.1648899999999998E-2</v>
       </c>
-      <c r="I16" s="59"/>
-      <c r="J16" s="51"/>
+      <c r="I16" s="51"/>
+      <c r="J16" s="55"/>
       <c r="K16" s="53"/>
     </row>
     <row r="17" spans="1:11">
-      <c r="A17" s="60">
+      <c r="A17" s="56">
         <v>12</v>
       </c>
-      <c r="B17" s="54" t="s">
+      <c r="B17" s="58" t="s">
         <v>23</v>
       </c>
       <c r="C17" s="44" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D17" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="E17" s="56" t="s">
-        <v>23</v>
-      </c>
-      <c r="F17" s="56" t="s">
-        <v>23</v>
-      </c>
-      <c r="G17" s="56" t="s">
+      <c r="E17" s="60" t="s">
+        <v>23</v>
+      </c>
+      <c r="F17" s="60" t="s">
+        <v>23</v>
+      </c>
+      <c r="G17" s="60" t="s">
         <v>23</v>
       </c>
       <c r="H17" s="45">
         <v>5.1855600000000002E-2</v>
       </c>
-      <c r="I17" s="58">
+      <c r="I17" s="50">
         <v>6.4500699999999994E-2</v>
       </c>
-      <c r="J17" s="50">
+      <c r="J17" s="54">
         <v>21</v>
       </c>
       <c r="K17" s="52"/>
     </row>
     <row r="18" spans="1:11">
-      <c r="A18" s="61"/>
-      <c r="B18" s="55"/>
+      <c r="A18" s="57"/>
+      <c r="B18" s="59"/>
       <c r="C18" s="46" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D18" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="E18" s="57"/>
-      <c r="F18" s="57"/>
-      <c r="G18" s="57"/>
+      <c r="E18" s="61"/>
+      <c r="F18" s="61"/>
+      <c r="G18" s="61"/>
       <c r="H18" s="47">
         <v>5.1648899999999998E-2</v>
       </c>
-      <c r="I18" s="59"/>
-      <c r="J18" s="51"/>
+      <c r="I18" s="51"/>
+      <c r="J18" s="55"/>
       <c r="K18" s="53"/>
     </row>
     <row r="19" spans="1:11" ht="78.75">
-      <c r="B19" s="54" t="s">
+      <c r="B19" s="58" t="s">
         <v>23</v>
       </c>
       <c r="C19" s="44" t="s">
+        <v>65</v>
+      </c>
+      <c r="D19" s="63" t="s">
+        <v>67</v>
+      </c>
+      <c r="E19" s="60" t="s">
+        <v>23</v>
+      </c>
+      <c r="F19" s="60" t="s">
+        <v>23</v>
+      </c>
+      <c r="G19" s="60" t="s">
+        <v>23</v>
+      </c>
+      <c r="H19" s="45" t="s">
         <v>66</v>
       </c>
-      <c r="D19" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="E19" s="56" t="s">
-        <v>23</v>
-      </c>
-      <c r="F19" s="56" t="s">
-        <v>23</v>
-      </c>
-      <c r="G19" s="56" t="s">
-        <v>23</v>
-      </c>
-      <c r="H19" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="I19" s="58">
+      <c r="I19" s="50">
         <v>6.4522999999999997E-2</v>
       </c>
-      <c r="J19" s="50"/>
+      <c r="J19" s="54"/>
       <c r="K19" s="52">
         <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:11">
-      <c r="B20" s="55"/>
+      <c r="B20" s="59"/>
       <c r="C20" s="46" t="s">
+        <v>64</v>
+      </c>
+      <c r="D20" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="E20" s="61"/>
+      <c r="F20" s="61"/>
+      <c r="G20" s="61"/>
+      <c r="H20" s="49"/>
+      <c r="I20" s="51"/>
+      <c r="J20" s="55"/>
+      <c r="K20" s="53"/>
+    </row>
+    <row r="21" spans="1:11" ht="25.5">
+      <c r="B21" s="58" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" s="44" t="s">
         <v>65</v>
       </c>
-      <c r="D20" s="46" t="s">
-        <v>23</v>
-      </c>
-      <c r="E20" s="57"/>
-      <c r="F20" s="57"/>
-      <c r="G20" s="57"/>
-      <c r="H20" s="49"/>
-      <c r="I20" s="59"/>
-      <c r="J20" s="51"/>
-      <c r="K20" s="53"/>
-    </row>
-    <row r="21" spans="1:11">
-      <c r="B21" s="54" t="s">
-        <v>23</v>
-      </c>
-      <c r="C21" s="44" t="s">
-        <v>66</v>
-      </c>
       <c r="D21" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="E21" s="56" t="s">
-        <v>23</v>
-      </c>
-      <c r="F21" s="56" t="s">
-        <v>23</v>
-      </c>
-      <c r="G21" s="56" t="s">
-        <v>23</v>
-      </c>
-      <c r="H21" s="45"/>
-      <c r="I21" s="58"/>
-      <c r="J21" s="50"/>
-      <c r="K21" s="52"/>
+      <c r="E21" s="60" t="s">
+        <v>68</v>
+      </c>
+      <c r="F21" s="60" t="s">
+        <v>22</v>
+      </c>
+      <c r="G21" s="60" t="s">
+        <v>70</v>
+      </c>
+      <c r="H21" s="45" t="s">
+        <v>69</v>
+      </c>
+      <c r="I21" s="50">
+        <v>4.496E-2</v>
+      </c>
+      <c r="J21" s="54"/>
+      <c r="K21" s="52">
+        <v>13</v>
+      </c>
     </row>
     <row r="22" spans="1:11">
-      <c r="B22" s="55"/>
+      <c r="B22" s="59"/>
       <c r="C22" s="46" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D22" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="E22" s="57"/>
-      <c r="F22" s="57"/>
-      <c r="G22" s="57"/>
+      <c r="E22" s="61"/>
+      <c r="F22" s="61"/>
+      <c r="G22" s="61"/>
       <c r="H22" s="49"/>
-      <c r="I22" s="59"/>
-      <c r="J22" s="51"/>
+      <c r="I22" s="51"/>
+      <c r="J22" s="55"/>
       <c r="K22" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="I17:I18"/>
-    <mergeCell ref="K17:K18"/>
-    <mergeCell ref="J13:J14"/>
-    <mergeCell ref="J15:J16"/>
-    <mergeCell ref="J17:J18"/>
-    <mergeCell ref="K13:K14"/>
-    <mergeCell ref="I15:I16"/>
-    <mergeCell ref="K15:K16"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="G17:G18"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="G13:G14"/>
     <mergeCell ref="J19:J20"/>
     <mergeCell ref="K19:K20"/>
     <mergeCell ref="B21:B22"/>
@@ -1672,6 +1666,30 @@
     <mergeCell ref="F19:F20"/>
     <mergeCell ref="G19:G20"/>
     <mergeCell ref="I19:I20"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="G17:G18"/>
+    <mergeCell ref="I17:I18"/>
+    <mergeCell ref="K17:K18"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="J15:J16"/>
+    <mergeCell ref="J17:J18"/>
+    <mergeCell ref="K13:K14"/>
+    <mergeCell ref="I15:I16"/>
+    <mergeCell ref="K15:K16"/>
+    <mergeCell ref="I13:I14"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="I1:J3 I23:J1048576 I4:I22">

</xml_diff>

<commit_message>
* Updated training results.
</commit_message>
<xml_diff>
--- a/training_result.xlsx
+++ b/training_result.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="13965" yWindow="0" windowWidth="18690" windowHeight="11685" activeTab="1"/>
+    <workbookView xWindow="16425" yWindow="0" windowWidth="18690" windowHeight="11685"/>
   </bookViews>
   <sheets>
     <sheet name="kernel_private" sheetId="6" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="89">
   <si>
     <t>Model</t>
   </si>
@@ -311,6 +311,58 @@
   </si>
   <si>
     <t>forked from the original version: Simple LGBM model (LB 0.0643922)</t>
+  </si>
+  <si>
+    <t>+ add fts: year
++ re-removed fts with low correlation</t>
+  </si>
+  <si>
+    <t>+boost_round: 475</t>
+  </si>
+  <si>
+    <t>2016 &amp; 2017</t>
+  </si>
+  <si>
+    <t>+ eta: 0.025
++ max_depth: 6
++ child_weight: 2
++ subsample: 0.8
++ bytree: 0.8
++ lambda: 10.0
++ alpha: 1.6
++ boost_round: 474</t>
+  </si>
+  <si>
+    <t>0.051477/474</t>
+  </si>
+  <si>
+    <t>-
++ 2017: structuretaxvaluedollacnt, landtaxvaluedollarcnt, taxvaluedollarcnt, taxamoun ==&gt; nan</t>
+  </si>
+  <si>
+    <t>0.051522/474</t>
+  </si>
+  <si>
+    <t>+ as 17
++ logerror: [-0.4, 0.4]</t>
+  </si>
+  <si>
+    <t>0.051151/474</t>
+  </si>
+  <si>
+    <t>+ max_depth: 100
++ num_leaves: 32
++ feature_fraction: 0.85
++ bagging_fraction: 0.95
++ bagging_freq: 8
++ learning_rate: 0.025
++ verbosity: 0</t>
+  </si>
+  <si>
+    <t>0.0516188/2930</t>
+  </si>
+  <si>
+    <t>as 17</t>
   </si>
 </sst>
 </file>
@@ -412,7 +464,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -534,11 +586,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -606,9 +695,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -645,113 +731,187 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="7">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1054,11 +1214,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L24"/>
+  <dimension ref="A1:L36"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I33" sqref="I33:I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1066,20 +1226,20 @@
     <col min="1" max="1" width="6" style="17" customWidth="1"/>
     <col min="2" max="2" width="65.28515625" style="17" customWidth="1"/>
     <col min="3" max="3" width="13" style="17" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" style="17" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" style="17" customWidth="1"/>
     <col min="5" max="5" width="10.85546875" style="17" customWidth="1"/>
     <col min="6" max="6" width="8.42578125" style="17" customWidth="1"/>
     <col min="7" max="7" width="12" style="17" customWidth="1"/>
     <col min="8" max="8" width="11.85546875" style="17" customWidth="1"/>
     <col min="9" max="9" width="11.28515625" style="17" customWidth="1"/>
-    <col min="10" max="10" width="7.140625" style="26" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="25" customWidth="1"/>
     <col min="11" max="11" width="8.28515625" style="17" customWidth="1"/>
     <col min="12" max="16384" width="9.140625" style="17"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="22" customFormat="1" ht="27.75" customHeight="1">
       <c r="A1" s="21"/>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="24" t="s">
         <v>71</v>
       </c>
       <c r="C1" s="21"/>
@@ -1102,7 +1262,7 @@
       <c r="G2" s="19"/>
       <c r="H2" s="19"/>
       <c r="I2" s="19"/>
-      <c r="J2" s="27"/>
+      <c r="J2" s="26"/>
       <c r="K2" s="19"/>
     </row>
     <row r="3" spans="1:12" ht="30" customHeight="1">
@@ -1133,7 +1293,7 @@
       <c r="I3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="J3" s="48" t="s">
+      <c r="J3" s="4" t="s">
         <v>62</v>
       </c>
       <c r="K3" s="5" t="s">
@@ -1141,619 +1301,963 @@
       </c>
     </row>
     <row r="4" spans="1:12" s="19" customFormat="1" ht="78.75">
-      <c r="A4" s="28">
+      <c r="A4" s="27">
         <v>1</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="59" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="30" t="s">
+      <c r="C4" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="29" t="s">
+      <c r="D4" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="31" t="s">
+      <c r="E4" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="F4" s="32" t="s">
+      <c r="F4" s="73" t="s">
         <v>31</v>
       </c>
-      <c r="G4" s="32" t="s">
+      <c r="G4" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="H4" s="32">
+      <c r="H4" s="73">
         <v>5.1650000000000001E-2</v>
       </c>
-      <c r="I4" s="33">
+      <c r="I4" s="32">
         <v>6.4611000000000002E-2</v>
       </c>
-      <c r="J4" s="32">
+      <c r="J4" s="73">
         <v>2</v>
       </c>
-      <c r="K4" s="34"/>
+      <c r="K4" s="33"/>
     </row>
     <row r="5" spans="1:12" s="19" customFormat="1" ht="33.75">
       <c r="A5" s="19">
         <v>2</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="60" t="s">
         <v>36</v>
       </c>
       <c r="C5" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="66" t="s">
         <v>23</v>
       </c>
       <c r="E5" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="18" t="s">
+      <c r="F5" s="66" t="s">
         <v>23</v>
       </c>
       <c r="G5" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="H5" s="18">
+      <c r="H5" s="66">
         <v>5.1652999999999998E-2</v>
       </c>
-      <c r="I5" s="33">
+      <c r="I5" s="32">
         <v>6.4565600000000001E-2</v>
       </c>
-      <c r="J5" s="32">
+      <c r="J5" s="73">
         <v>3</v>
       </c>
-      <c r="K5" s="34"/>
+      <c r="K5" s="33"/>
     </row>
     <row r="6" spans="1:12" ht="67.5">
-      <c r="A6" s="35">
+      <c r="A6" s="34">
         <v>3</v>
       </c>
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="61" t="s">
         <v>41</v>
       </c>
-      <c r="C6" s="37" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="29" t="s">
+      <c r="C6" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="59" t="s">
         <v>40</v>
       </c>
-      <c r="E6" s="37" t="s">
+      <c r="E6" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="F6" s="37" t="s">
+      <c r="F6" s="74" t="s">
         <v>39</v>
       </c>
-      <c r="G6" s="37" t="s">
-        <v>23</v>
-      </c>
-      <c r="H6" s="37">
+      <c r="G6" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6" s="74">
         <v>5.1644000000000002E-2</v>
       </c>
-      <c r="I6" s="33">
+      <c r="I6" s="32">
         <v>6.4564800000000006E-2</v>
       </c>
-      <c r="J6" s="32">
+      <c r="J6" s="73">
         <v>7</v>
       </c>
-      <c r="K6" s="34"/>
+      <c r="K6" s="33"/>
     </row>
     <row r="7" spans="1:12" ht="33.75">
-      <c r="A7" s="35">
+      <c r="A7" s="34">
         <v>4</v>
       </c>
-      <c r="B7" s="36" t="s">
+      <c r="B7" s="61" t="s">
         <v>42</v>
       </c>
-      <c r="C7" s="37" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="29" t="s">
+      <c r="C7" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="59" t="s">
         <v>38</v>
       </c>
-      <c r="E7" s="37" t="s">
+      <c r="E7" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="F7" s="37" t="s">
+      <c r="F7" s="74" t="s">
         <v>38</v>
       </c>
-      <c r="G7" s="37" t="s">
-        <v>23</v>
-      </c>
-      <c r="H7" s="37">
+      <c r="G7" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7" s="74">
         <v>5.1604999999999998E-2</v>
       </c>
-      <c r="I7" s="33">
+      <c r="I7" s="32">
         <v>6.4559000000000005E-2</v>
       </c>
-      <c r="J7" s="32">
+      <c r="J7" s="73">
         <v>8</v>
       </c>
-      <c r="K7" s="34"/>
+      <c r="K7" s="33"/>
     </row>
     <row r="8" spans="1:12" ht="33.75">
-      <c r="A8" s="35">
+      <c r="A8" s="34">
         <v>5</v>
       </c>
-      <c r="B8" s="36" t="s">
+      <c r="B8" s="61" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="37" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="29" t="s">
+      <c r="C8" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="59" t="s">
         <v>38</v>
       </c>
-      <c r="E8" s="37" t="s">
+      <c r="E8" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="F8" s="37" t="s">
+      <c r="F8" s="74" t="s">
         <v>38</v>
       </c>
-      <c r="G8" s="37" t="s">
-        <v>23</v>
-      </c>
-      <c r="H8" s="38">
+      <c r="G8" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="H8" s="77">
         <v>5.1681999999999999E-2</v>
       </c>
-      <c r="I8" s="33">
+      <c r="I8" s="32">
         <v>6.4625600000000005E-2</v>
       </c>
-      <c r="J8" s="38">
+      <c r="J8" s="77">
         <v>9</v>
       </c>
-      <c r="K8" s="39"/>
-      <c r="L8" s="24" t="s">
+      <c r="K8" s="36"/>
+      <c r="L8" s="23" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="45">
-      <c r="A9" s="35">
+      <c r="A9" s="34">
         <v>6</v>
       </c>
-      <c r="B9" s="36" t="s">
+      <c r="B9" s="61" t="s">
         <v>45</v>
       </c>
-      <c r="C9" s="37" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="29" t="s">
+      <c r="C9" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="59" t="s">
         <v>38</v>
       </c>
-      <c r="E9" s="37" t="s">
+      <c r="E9" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="F9" s="37" t="s">
+      <c r="F9" s="74" t="s">
         <v>38</v>
       </c>
-      <c r="G9" s="37" t="s">
-        <v>23</v>
-      </c>
-      <c r="H9" s="38">
+      <c r="G9" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="H9" s="77">
         <v>5.1711E-2</v>
       </c>
-      <c r="I9" s="33">
+      <c r="I9" s="32">
         <v>6.4605700000000002E-2</v>
       </c>
-      <c r="J9" s="38">
+      <c r="J9" s="77">
         <v>11</v>
       </c>
-      <c r="K9" s="39"/>
+      <c r="K9" s="36"/>
     </row>
     <row r="10" spans="1:12" ht="45">
-      <c r="A10" s="35">
+      <c r="A10" s="34">
         <v>7</v>
       </c>
-      <c r="B10" s="36" t="s">
+      <c r="B10" s="61" t="s">
         <v>47</v>
       </c>
-      <c r="C10" s="37" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10" s="29" t="s">
+      <c r="C10" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="59" t="s">
         <v>38</v>
       </c>
-      <c r="E10" s="37" t="s">
+      <c r="E10" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="F10" s="37" t="s">
+      <c r="F10" s="74" t="s">
         <v>51</v>
       </c>
-      <c r="G10" s="32" t="s">
+      <c r="G10" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="H10" s="38">
+      <c r="H10" s="77">
         <v>5.1580000000000001E-2</v>
       </c>
-      <c r="I10" s="33">
+      <c r="I10" s="32">
         <v>6.4518699999999998E-2</v>
       </c>
-      <c r="J10" s="38">
+      <c r="J10" s="77">
         <v>12</v>
       </c>
-      <c r="K10" s="39"/>
-      <c r="L10" s="24" t="s">
+      <c r="K10" s="36"/>
+      <c r="L10" s="23" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="123.75">
-      <c r="A11" s="40">
+      <c r="A11" s="37">
         <v>8</v>
       </c>
-      <c r="B11" s="41" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="37" t="s">
+      <c r="B11" s="62" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="D11" s="29" t="s">
+      <c r="D11" s="59" t="s">
         <v>49</v>
       </c>
-      <c r="E11" s="37" t="s">
-        <v>23</v>
-      </c>
-      <c r="F11" s="37" t="s">
-        <v>23</v>
-      </c>
-      <c r="G11" s="37" t="s">
-        <v>23</v>
-      </c>
-      <c r="H11" s="38">
+      <c r="E11" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" s="74" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="H11" s="77">
         <v>0.51668700000000001</v>
       </c>
-      <c r="I11" s="42">
+      <c r="I11" s="38">
         <v>6.4663100000000001E-2</v>
       </c>
-      <c r="J11" s="38">
+      <c r="J11" s="77">
         <v>15</v>
       </c>
-      <c r="K11" s="39"/>
+      <c r="K11" s="36"/>
     </row>
     <row r="12" spans="1:12" ht="25.5">
-      <c r="A12" s="40">
+      <c r="A12" s="37">
         <v>9</v>
       </c>
-      <c r="B12" s="43" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" s="43" t="s">
+      <c r="B12" s="63" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="39" t="s">
         <v>53</v>
       </c>
-      <c r="D12" s="43" t="s">
-        <v>23</v>
-      </c>
-      <c r="E12" s="37" t="s">
-        <v>23</v>
-      </c>
-      <c r="F12" s="37" t="s">
-        <v>23</v>
-      </c>
-      <c r="G12" s="37" t="s">
-        <v>23</v>
-      </c>
-      <c r="H12" s="37" t="s">
+      <c r="D12" s="63" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" s="74" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="H12" s="74" t="s">
         <v>54</v>
       </c>
-      <c r="I12" s="42">
+      <c r="I12" s="38">
         <v>6.4527600000000004E-2</v>
       </c>
-      <c r="J12" s="32">
+      <c r="J12" s="73">
         <v>16</v>
       </c>
-      <c r="K12" s="34"/>
+      <c r="K12" s="33"/>
     </row>
     <row r="13" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A13" s="57">
+      <c r="A13" s="54">
         <v>10</v>
       </c>
-      <c r="B13" s="65" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13" s="44" t="s">
+      <c r="B13" s="64" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="40" t="s">
         <v>55</v>
       </c>
-      <c r="D13" s="44" t="s">
-        <v>23</v>
-      </c>
-      <c r="E13" s="67" t="s">
-        <v>23</v>
-      </c>
-      <c r="F13" s="67" t="s">
-        <v>23</v>
-      </c>
-      <c r="G13" s="67" t="s">
-        <v>23</v>
-      </c>
-      <c r="H13" s="45">
+      <c r="D13" s="67" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="56" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="75" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13" s="56" t="s">
+        <v>23</v>
+      </c>
+      <c r="H13" s="78">
         <v>5.1580000000000001E-2</v>
       </c>
-      <c r="I13" s="59">
+      <c r="I13" s="50">
         <v>6.4497299999999994E-2</v>
       </c>
-      <c r="J13" s="63">
+      <c r="J13" s="80">
         <v>17</v>
       </c>
-      <c r="K13" s="61"/>
+      <c r="K13" s="52"/>
     </row>
     <row r="14" spans="1:12">
-      <c r="A14" s="58"/>
-      <c r="B14" s="66"/>
-      <c r="C14" s="46" t="s">
+      <c r="A14" s="55"/>
+      <c r="B14" s="65"/>
+      <c r="C14" s="41" t="s">
         <v>57</v>
       </c>
-      <c r="D14" s="46" t="s">
+      <c r="D14" s="68" t="s">
         <v>56</v>
       </c>
-      <c r="E14" s="68"/>
-      <c r="F14" s="68"/>
-      <c r="G14" s="68"/>
-      <c r="H14" s="47">
+      <c r="E14" s="57"/>
+      <c r="F14" s="76"/>
+      <c r="G14" s="57"/>
+      <c r="H14" s="79">
         <v>5.1648899999999998E-2</v>
       </c>
-      <c r="I14" s="60"/>
-      <c r="J14" s="64"/>
-      <c r="K14" s="62"/>
+      <c r="I14" s="51"/>
+      <c r="J14" s="81"/>
+      <c r="K14" s="53"/>
     </row>
     <row r="15" spans="1:12">
-      <c r="A15" s="57">
+      <c r="A15" s="54">
         <v>11</v>
       </c>
-      <c r="B15" s="65" t="s">
-        <v>23</v>
-      </c>
-      <c r="C15" s="44" t="s">
+      <c r="B15" s="64" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="40" t="s">
         <v>58</v>
       </c>
-      <c r="D15" s="44" t="s">
-        <v>23</v>
-      </c>
-      <c r="E15" s="67" t="s">
-        <v>23</v>
-      </c>
-      <c r="F15" s="67" t="s">
-        <v>23</v>
-      </c>
-      <c r="G15" s="67" t="s">
-        <v>23</v>
-      </c>
-      <c r="H15" s="45">
+      <c r="D15" s="67" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" s="56" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15" s="75" t="s">
+        <v>23</v>
+      </c>
+      <c r="G15" s="56" t="s">
+        <v>23</v>
+      </c>
+      <c r="H15" s="78">
         <v>5.1717800000000001E-2</v>
       </c>
-      <c r="I15" s="59">
+      <c r="I15" s="50">
         <v>6.4495999999999998E-2</v>
       </c>
-      <c r="J15" s="63">
+      <c r="J15" s="80">
         <v>20</v>
       </c>
-      <c r="K15" s="61"/>
+      <c r="K15" s="52"/>
     </row>
     <row r="16" spans="1:12">
-      <c r="A16" s="58"/>
-      <c r="B16" s="66"/>
-      <c r="C16" s="46" t="s">
+      <c r="A16" s="55"/>
+      <c r="B16" s="65"/>
+      <c r="C16" s="41" t="s">
         <v>59</v>
       </c>
-      <c r="D16" s="46" t="s">
-        <v>23</v>
-      </c>
-      <c r="E16" s="68"/>
-      <c r="F16" s="68"/>
-      <c r="G16" s="68"/>
-      <c r="H16" s="47">
+      <c r="D16" s="68" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" s="57"/>
+      <c r="F16" s="76"/>
+      <c r="G16" s="57"/>
+      <c r="H16" s="79">
         <v>5.1648899999999998E-2</v>
       </c>
-      <c r="I16" s="60"/>
-      <c r="J16" s="64"/>
-      <c r="K16" s="62"/>
+      <c r="I16" s="51"/>
+      <c r="J16" s="81"/>
+      <c r="K16" s="53"/>
     </row>
     <row r="17" spans="1:12">
-      <c r="A17" s="57">
+      <c r="A17" s="54">
         <v>12</v>
       </c>
-      <c r="B17" s="65" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" s="44" t="s">
+      <c r="B17" s="64" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="40" t="s">
         <v>60</v>
       </c>
-      <c r="D17" s="44" t="s">
-        <v>23</v>
-      </c>
-      <c r="E17" s="67" t="s">
-        <v>23</v>
-      </c>
-      <c r="F17" s="67" t="s">
-        <v>23</v>
-      </c>
-      <c r="G17" s="67" t="s">
-        <v>23</v>
-      </c>
-      <c r="H17" s="45">
+      <c r="D17" s="67" t="s">
+        <v>23</v>
+      </c>
+      <c r="E17" s="56" t="s">
+        <v>23</v>
+      </c>
+      <c r="F17" s="75" t="s">
+        <v>23</v>
+      </c>
+      <c r="G17" s="56" t="s">
+        <v>23</v>
+      </c>
+      <c r="H17" s="78">
         <v>5.1855600000000002E-2</v>
       </c>
-      <c r="I17" s="59">
+      <c r="I17" s="50">
         <v>6.4500699999999994E-2</v>
       </c>
-      <c r="J17" s="63">
+      <c r="J17" s="80">
         <v>21</v>
       </c>
-      <c r="K17" s="61"/>
+      <c r="K17" s="52"/>
     </row>
     <row r="18" spans="1:12">
-      <c r="A18" s="58"/>
-      <c r="B18" s="66"/>
-      <c r="C18" s="46" t="s">
+      <c r="A18" s="55"/>
+      <c r="B18" s="65"/>
+      <c r="C18" s="41" t="s">
         <v>61</v>
       </c>
-      <c r="D18" s="46" t="s">
-        <v>23</v>
-      </c>
-      <c r="E18" s="68"/>
-      <c r="F18" s="68"/>
-      <c r="G18" s="68"/>
-      <c r="H18" s="47">
+      <c r="D18" s="68" t="s">
+        <v>23</v>
+      </c>
+      <c r="E18" s="57"/>
+      <c r="F18" s="76"/>
+      <c r="G18" s="57"/>
+      <c r="H18" s="79">
         <v>5.1648899999999998E-2</v>
       </c>
-      <c r="I18" s="60"/>
-      <c r="J18" s="64"/>
-      <c r="K18" s="62"/>
+      <c r="I18" s="51"/>
+      <c r="J18" s="81"/>
+      <c r="K18" s="53"/>
     </row>
     <row r="19" spans="1:12" ht="78.75">
-      <c r="A19" s="57">
+      <c r="A19" s="54">
         <v>13</v>
       </c>
-      <c r="B19" s="65" t="s">
-        <v>23</v>
-      </c>
-      <c r="C19" s="44" t="s">
+      <c r="B19" s="64" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="40" t="s">
         <v>65</v>
       </c>
-      <c r="D19" s="50" t="s">
+      <c r="D19" s="69" t="s">
         <v>67</v>
       </c>
-      <c r="E19" s="67" t="s">
-        <v>23</v>
-      </c>
-      <c r="F19" s="67" t="s">
-        <v>23</v>
-      </c>
-      <c r="G19" s="67" t="s">
-        <v>23</v>
-      </c>
-      <c r="H19" s="45" t="s">
+      <c r="E19" s="56" t="s">
+        <v>23</v>
+      </c>
+      <c r="F19" s="75" t="s">
+        <v>23</v>
+      </c>
+      <c r="G19" s="56" t="s">
+        <v>23</v>
+      </c>
+      <c r="H19" s="78" t="s">
         <v>66</v>
       </c>
-      <c r="I19" s="59">
+      <c r="I19" s="50">
         <v>6.4522999999999997E-2</v>
       </c>
-      <c r="J19" s="63"/>
-      <c r="K19" s="61">
+      <c r="J19" s="80"/>
+      <c r="K19" s="52">
         <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:12">
-      <c r="A20" s="58"/>
-      <c r="B20" s="66"/>
-      <c r="C20" s="46" t="s">
+      <c r="A20" s="55"/>
+      <c r="B20" s="65"/>
+      <c r="C20" s="41" t="s">
         <v>64</v>
       </c>
-      <c r="D20" s="46" t="s">
-        <v>23</v>
-      </c>
-      <c r="E20" s="68"/>
-      <c r="F20" s="68"/>
-      <c r="G20" s="68"/>
-      <c r="H20" s="49"/>
-      <c r="I20" s="60"/>
-      <c r="J20" s="64"/>
-      <c r="K20" s="62"/>
+      <c r="D20" s="68" t="s">
+        <v>23</v>
+      </c>
+      <c r="E20" s="57"/>
+      <c r="F20" s="76"/>
+      <c r="G20" s="57"/>
+      <c r="H20" s="79"/>
+      <c r="I20" s="51"/>
+      <c r="J20" s="81"/>
+      <c r="K20" s="53"/>
     </row>
     <row r="21" spans="1:12" ht="25.5">
-      <c r="A21" s="57">
+      <c r="A21" s="54">
         <v>14</v>
       </c>
-      <c r="B21" s="65" t="s">
-        <v>23</v>
-      </c>
-      <c r="C21" s="44" t="s">
+      <c r="B21" s="64" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" s="40" t="s">
         <v>65</v>
       </c>
-      <c r="D21" s="44" t="s">
-        <v>23</v>
-      </c>
-      <c r="E21" s="67" t="s">
+      <c r="D21" s="67" t="s">
+        <v>23</v>
+      </c>
+      <c r="E21" s="56" t="s">
         <v>68</v>
       </c>
-      <c r="F21" s="67" t="s">
+      <c r="F21" s="75" t="s">
         <v>22</v>
       </c>
-      <c r="G21" s="67" t="s">
+      <c r="G21" s="56" t="s">
         <v>70</v>
       </c>
-      <c r="H21" s="45" t="s">
+      <c r="H21" s="78" t="s">
         <v>69</v>
       </c>
-      <c r="I21" s="59">
+      <c r="I21" s="50">
         <v>6.4495999999999998E-2</v>
       </c>
-      <c r="J21" s="63"/>
-      <c r="K21" s="61">
+      <c r="J21" s="80"/>
+      <c r="K21" s="52">
         <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:12">
-      <c r="A22" s="58"/>
-      <c r="B22" s="66"/>
-      <c r="C22" s="46" t="s">
+      <c r="A22" s="55"/>
+      <c r="B22" s="65"/>
+      <c r="C22" s="41" t="s">
         <v>64</v>
       </c>
-      <c r="D22" s="46" t="s">
-        <v>23</v>
-      </c>
-      <c r="E22" s="68"/>
-      <c r="F22" s="68"/>
-      <c r="G22" s="68"/>
-      <c r="H22" s="49"/>
-      <c r="I22" s="60"/>
-      <c r="J22" s="64"/>
-      <c r="K22" s="62"/>
+      <c r="D22" s="68" t="s">
+        <v>23</v>
+      </c>
+      <c r="E22" s="57"/>
+      <c r="F22" s="76"/>
+      <c r="G22" s="57"/>
+      <c r="H22" s="79"/>
+      <c r="I22" s="51"/>
+      <c r="J22" s="81"/>
+      <c r="K22" s="53"/>
     </row>
     <row r="23" spans="1:12">
-      <c r="A23" s="57">
+      <c r="A23" s="54">
         <v>15</v>
       </c>
-      <c r="B23" s="65" t="s">
-        <v>23</v>
-      </c>
-      <c r="C23" s="52" t="s">
+      <c r="B23" s="64" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" s="43" t="s">
         <v>65</v>
       </c>
-      <c r="D23" s="55" t="s">
+      <c r="D23" s="70" t="s">
         <v>73</v>
       </c>
-      <c r="E23" s="67" t="s">
-        <v>23</v>
-      </c>
-      <c r="F23" s="67" t="s">
+      <c r="E23" s="56" t="s">
+        <v>23</v>
+      </c>
+      <c r="F23" s="75" t="s">
         <v>22</v>
       </c>
-      <c r="G23" s="67" t="s">
+      <c r="G23" s="56" t="s">
         <v>70</v>
       </c>
-      <c r="H23" s="54" t="s">
+      <c r="H23" s="78" t="s">
         <v>74</v>
       </c>
-      <c r="I23" s="59">
+      <c r="I23" s="50">
         <v>6.7741899999999994E-2</v>
       </c>
-      <c r="J23" s="63"/>
-      <c r="K23" s="61">
+      <c r="J23" s="80"/>
+      <c r="K23" s="52">
         <v>16</v>
       </c>
-      <c r="L23" s="24" t="s">
+      <c r="L23" s="23" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="24" spans="1:12">
-      <c r="A24" s="58"/>
-      <c r="B24" s="66"/>
-      <c r="C24" s="53" t="s">
+      <c r="A24" s="55"/>
+      <c r="B24" s="65"/>
+      <c r="C24" s="44" t="s">
         <v>64</v>
       </c>
-      <c r="D24" s="53" t="s">
-        <v>23</v>
-      </c>
-      <c r="E24" s="68"/>
-      <c r="F24" s="68"/>
-      <c r="G24" s="68"/>
-      <c r="H24" s="51"/>
-      <c r="I24" s="60"/>
-      <c r="J24" s="64"/>
-      <c r="K24" s="62"/>
+      <c r="D24" s="68" t="s">
+        <v>23</v>
+      </c>
+      <c r="E24" s="57"/>
+      <c r="F24" s="76"/>
+      <c r="G24" s="57"/>
+      <c r="H24" s="79"/>
+      <c r="I24" s="51"/>
+      <c r="J24" s="81"/>
+      <c r="K24" s="53"/>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="A25" s="54">
+        <v>16</v>
+      </c>
+      <c r="B25" s="64" t="s">
+        <v>77</v>
+      </c>
+      <c r="C25" s="46" t="s">
+        <v>65</v>
+      </c>
+      <c r="D25" s="70" t="s">
+        <v>78</v>
+      </c>
+      <c r="E25" s="56" t="s">
+        <v>23</v>
+      </c>
+      <c r="F25" s="75" t="s">
+        <v>22</v>
+      </c>
+      <c r="G25" s="56" t="s">
+        <v>79</v>
+      </c>
+      <c r="H25" s="78">
+        <v>5.1631000000000003E-2</v>
+      </c>
+      <c r="I25" s="50">
+        <v>6.4437400000000006E-2</v>
+      </c>
+      <c r="J25" s="80">
+        <v>27</v>
+      </c>
+      <c r="K25" s="52"/>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="A26" s="55"/>
+      <c r="B26" s="65"/>
+      <c r="C26" s="47" t="s">
+        <v>64</v>
+      </c>
+      <c r="D26" s="68" t="s">
+        <v>23</v>
+      </c>
+      <c r="E26" s="57"/>
+      <c r="F26" s="76"/>
+      <c r="G26" s="57"/>
+      <c r="H26" s="79"/>
+      <c r="I26" s="51"/>
+      <c r="J26" s="81"/>
+      <c r="K26" s="53"/>
+    </row>
+    <row r="27" spans="1:12" ht="90">
+      <c r="A27" s="54">
+        <v>17</v>
+      </c>
+      <c r="B27" s="64" t="s">
+        <v>23</v>
+      </c>
+      <c r="C27" s="48" t="s">
+        <v>65</v>
+      </c>
+      <c r="D27" s="69" t="s">
+        <v>80</v>
+      </c>
+      <c r="E27" s="56" t="s">
+        <v>23</v>
+      </c>
+      <c r="F27" s="75" t="s">
+        <v>22</v>
+      </c>
+      <c r="G27" s="56" t="s">
+        <v>79</v>
+      </c>
+      <c r="H27" s="78" t="s">
+        <v>81</v>
+      </c>
+      <c r="I27" s="50">
+        <v>6.4374500000000001E-2</v>
+      </c>
+      <c r="J27" s="80">
+        <v>28</v>
+      </c>
+      <c r="K27" s="52"/>
+    </row>
+    <row r="28" spans="1:12">
+      <c r="A28" s="55"/>
+      <c r="B28" s="65"/>
+      <c r="C28" s="49" t="s">
+        <v>64</v>
+      </c>
+      <c r="D28" s="68" t="s">
+        <v>23</v>
+      </c>
+      <c r="E28" s="57"/>
+      <c r="F28" s="76"/>
+      <c r="G28" s="57"/>
+      <c r="H28" s="79"/>
+      <c r="I28" s="51"/>
+      <c r="J28" s="81"/>
+      <c r="K28" s="53"/>
+    </row>
+    <row r="29" spans="1:12" ht="25.5">
+      <c r="A29" s="54">
+        <v>18</v>
+      </c>
+      <c r="B29" s="64" t="s">
+        <v>82</v>
+      </c>
+      <c r="C29" s="48" t="s">
+        <v>65</v>
+      </c>
+      <c r="D29" s="71" t="s">
+        <v>23</v>
+      </c>
+      <c r="E29" s="56" t="s">
+        <v>23</v>
+      </c>
+      <c r="F29" s="75" t="s">
+        <v>22</v>
+      </c>
+      <c r="G29" s="56" t="s">
+        <v>79</v>
+      </c>
+      <c r="H29" s="78" t="s">
+        <v>83</v>
+      </c>
+      <c r="I29" s="50">
+        <v>6.4544000000000004E-2</v>
+      </c>
+      <c r="J29" s="80">
+        <v>29</v>
+      </c>
+      <c r="K29" s="52"/>
+    </row>
+    <row r="30" spans="1:12">
+      <c r="A30" s="55"/>
+      <c r="B30" s="65"/>
+      <c r="C30" s="49" t="s">
+        <v>64</v>
+      </c>
+      <c r="D30" s="68" t="s">
+        <v>23</v>
+      </c>
+      <c r="E30" s="57"/>
+      <c r="F30" s="76"/>
+      <c r="G30" s="57"/>
+      <c r="H30" s="79"/>
+      <c r="I30" s="51"/>
+      <c r="J30" s="81"/>
+      <c r="K30" s="53"/>
+    </row>
+    <row r="31" spans="1:12" ht="25.5">
+      <c r="A31" s="54">
+        <v>19</v>
+      </c>
+      <c r="B31" s="64" t="s">
+        <v>84</v>
+      </c>
+      <c r="C31" s="48" t="s">
+        <v>65</v>
+      </c>
+      <c r="D31" s="71" t="s">
+        <v>23</v>
+      </c>
+      <c r="E31" s="56" t="s">
+        <v>23</v>
+      </c>
+      <c r="F31" s="75" t="s">
+        <v>22</v>
+      </c>
+      <c r="G31" s="56" t="s">
+        <v>79</v>
+      </c>
+      <c r="H31" s="78" t="s">
+        <v>85</v>
+      </c>
+      <c r="I31" s="50">
+        <v>6.4513699999999993E-2</v>
+      </c>
+      <c r="J31" s="80">
+        <v>30</v>
+      </c>
+      <c r="K31" s="52"/>
+    </row>
+    <row r="32" spans="1:12">
+      <c r="A32" s="55"/>
+      <c r="B32" s="65"/>
+      <c r="C32" s="49" t="s">
+        <v>64</v>
+      </c>
+      <c r="D32" s="68" t="s">
+        <v>23</v>
+      </c>
+      <c r="E32" s="57"/>
+      <c r="F32" s="76"/>
+      <c r="G32" s="57"/>
+      <c r="H32" s="79"/>
+      <c r="I32" s="51"/>
+      <c r="J32" s="81"/>
+      <c r="K32" s="53"/>
+    </row>
+    <row r="33" spans="1:11" ht="25.5">
+      <c r="A33" s="54">
+        <v>20</v>
+      </c>
+      <c r="B33" s="64" t="s">
+        <v>88</v>
+      </c>
+      <c r="C33" s="48" t="s">
+        <v>58</v>
+      </c>
+      <c r="D33" s="71" t="s">
+        <v>23</v>
+      </c>
+      <c r="E33" s="56" t="s">
+        <v>23</v>
+      </c>
+      <c r="F33" s="75" t="s">
+        <v>22</v>
+      </c>
+      <c r="G33" s="56" t="s">
+        <v>79</v>
+      </c>
+      <c r="H33" s="78" t="s">
+        <v>81</v>
+      </c>
+      <c r="I33" s="50">
+        <v>6.4355200000000001E-2</v>
+      </c>
+      <c r="J33" s="80">
+        <v>32</v>
+      </c>
+      <c r="K33" s="52"/>
+    </row>
+    <row r="34" spans="1:11" ht="78.75">
+      <c r="A34" s="55"/>
+      <c r="B34" s="65"/>
+      <c r="C34" s="49" t="s">
+        <v>59</v>
+      </c>
+      <c r="D34" s="72" t="s">
+        <v>86</v>
+      </c>
+      <c r="E34" s="57"/>
+      <c r="F34" s="76"/>
+      <c r="G34" s="57"/>
+      <c r="H34" s="79" t="s">
+        <v>87</v>
+      </c>
+      <c r="I34" s="51"/>
+      <c r="J34" s="81"/>
+      <c r="K34" s="53"/>
+    </row>
+    <row r="35" spans="1:11" ht="25.5">
+      <c r="A35" s="54">
+        <v>21</v>
+      </c>
+      <c r="B35" s="64" t="s">
+        <v>88</v>
+      </c>
+      <c r="C35" s="48" t="s">
+        <v>60</v>
+      </c>
+      <c r="D35" s="71" t="s">
+        <v>23</v>
+      </c>
+      <c r="E35" s="56" t="s">
+        <v>23</v>
+      </c>
+      <c r="F35" s="75" t="s">
+        <v>22</v>
+      </c>
+      <c r="G35" s="56" t="s">
+        <v>79</v>
+      </c>
+      <c r="H35" s="78" t="s">
+        <v>81</v>
+      </c>
+      <c r="I35" s="50">
+        <v>6.4361000000000002E-2</v>
+      </c>
+      <c r="J35" s="80">
+        <v>33</v>
+      </c>
+      <c r="K35" s="52"/>
+    </row>
+    <row r="36" spans="1:11" ht="25.5">
+      <c r="A36" s="55"/>
+      <c r="B36" s="65"/>
+      <c r="C36" s="49" t="s">
+        <v>61</v>
+      </c>
+      <c r="D36" s="68" t="s">
+        <v>23</v>
+      </c>
+      <c r="E36" s="57"/>
+      <c r="F36" s="76"/>
+      <c r="G36" s="57"/>
+      <c r="H36" s="79" t="s">
+        <v>87</v>
+      </c>
+      <c r="I36" s="51"/>
+      <c r="J36" s="81"/>
+      <c r="K36" s="53"/>
     </row>
   </sheetData>
-  <mergeCells count="48">
+  <mergeCells count="96">
+    <mergeCell ref="I35:I36"/>
+    <mergeCell ref="J35:J36"/>
+    <mergeCell ref="K35:K36"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="F35:F36"/>
+    <mergeCell ref="G35:G36"/>
+    <mergeCell ref="I31:I32"/>
+    <mergeCell ref="J31:J32"/>
+    <mergeCell ref="K31:K32"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="F33:F34"/>
+    <mergeCell ref="G33:G34"/>
+    <mergeCell ref="I33:I34"/>
+    <mergeCell ref="J33:J34"/>
+    <mergeCell ref="K33:K34"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="F31:F32"/>
+    <mergeCell ref="G31:G32"/>
+    <mergeCell ref="I27:I28"/>
+    <mergeCell ref="J27:J28"/>
+    <mergeCell ref="K27:K28"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="G29:G30"/>
+    <mergeCell ref="I29:I30"/>
+    <mergeCell ref="J29:J30"/>
+    <mergeCell ref="K29:K30"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="G27:G28"/>
     <mergeCell ref="I23:I24"/>
     <mergeCell ref="J23:J24"/>
     <mergeCell ref="K23:K24"/>
@@ -1802,10 +2306,18 @@
     <mergeCell ref="E17:E18"/>
     <mergeCell ref="F17:F18"/>
     <mergeCell ref="G17:G18"/>
+    <mergeCell ref="I25:I26"/>
+    <mergeCell ref="J25:J26"/>
+    <mergeCell ref="K25:K26"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="G25:G26"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="I1:J3 I25:J1048576 I4:I24">
-    <cfRule type="top10" dxfId="1" priority="1" bottom="1" rank="1"/>
+  <conditionalFormatting sqref="I1:J3 I37:J1048576 I4:I36">
+    <cfRule type="top10" dxfId="6" priority="1" bottom="1" rank="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1816,30 +2328,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomLeft" activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6" style="56" customWidth="1"/>
-    <col min="2" max="2" width="65.28515625" style="56" customWidth="1"/>
-    <col min="3" max="3" width="13" style="56" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" style="56" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" style="56" customWidth="1"/>
-    <col min="6" max="6" width="8.42578125" style="56" customWidth="1"/>
-    <col min="7" max="7" width="12" style="56" customWidth="1"/>
-    <col min="8" max="8" width="11.85546875" style="56" customWidth="1"/>
-    <col min="9" max="9" width="11.28515625" style="56" customWidth="1"/>
-    <col min="10" max="10" width="7.140625" style="56" customWidth="1"/>
-    <col min="11" max="11" width="8.28515625" style="56" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="56"/>
+    <col min="1" max="1" width="6" style="45" customWidth="1"/>
+    <col min="2" max="2" width="65.28515625" style="45" customWidth="1"/>
+    <col min="3" max="3" width="13" style="45" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" style="45" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" style="45" customWidth="1"/>
+    <col min="6" max="6" width="8.42578125" style="45" customWidth="1"/>
+    <col min="7" max="7" width="12" style="45" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" style="45" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" style="45" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="45" customWidth="1"/>
+    <col min="11" max="11" width="8.28515625" style="45" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="45"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="22" customFormat="1" ht="27.75" customHeight="1">
       <c r="A1" s="21"/>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="24" t="s">
         <v>75</v>
       </c>
       <c r="C1" s="21"/>
@@ -1853,17 +2365,17 @@
       <c r="K1" s="21"/>
     </row>
     <row r="2" spans="1:11" ht="2.25" customHeight="1">
-      <c r="A2" s="27"/>
+      <c r="A2" s="26"/>
       <c r="B2" s="16"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
-      <c r="K2" s="27"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
+      <c r="K2" s="26"/>
     </row>
     <row r="3" spans="1:11" ht="30" customHeight="1">
       <c r="A3" s="4" t="s">
@@ -1893,37 +2405,39 @@
       <c r="I3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="J3" s="48" t="s">
+      <c r="J3" s="42" t="s">
         <v>62</v>
       </c>
       <c r="K3" s="5" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="27" customFormat="1" ht="15.75">
-      <c r="A4" s="28">
+    <row r="4" spans="1:11" s="26" customFormat="1" ht="15.75">
+      <c r="A4" s="27">
         <v>1</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="C4" s="30" t="s">
+      <c r="C4" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="D4" s="29"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="32"/>
-      <c r="H4" s="32"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="32">
+      <c r="D4" s="28"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="32">
+        <v>6.4392199999999997E-2</v>
+      </c>
+      <c r="J4" s="31">
         <v>4</v>
       </c>
-      <c r="K4" s="34"/>
+      <c r="K4" s="33"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="I1:J3 I5:J1048576 I4">
-    <cfRule type="top10" dxfId="0" priority="2" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="5" priority="2" bottom="1" rank="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2203,10 +2717,10 @@
       <c r="D10" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="69" t="s">
+      <c r="E10" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="F10" s="69"/>
+      <c r="F10" s="58"/>
       <c r="G10" s="14" t="s">
         <v>23</v>
       </c>

</xml_diff>